<commit_message>
Open Git Bash Here in IntelliJ
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="36" windowWidth="22116" windowHeight="9552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="22110" windowHeight="9555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -858,13 +858,13 @@
     <t>Show tool window bar (if minimized)</t>
   </si>
   <si>
-    <t>Open Terminal Here</t>
-  </si>
-  <si>
     <t>Ctrl + Shift + H / Ctrl + Alt + H</t>
   </si>
   <si>
     <t>Method hierarchy / Call hierarchy</t>
+  </si>
+  <si>
+    <t>External Tools &gt; Git Bash</t>
   </si>
 </sst>
 </file>
@@ -1351,24 +1351,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.6640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="3.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="37.88671875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.88671875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3.33203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="37.5546875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.5546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.44140625" style="2"/>
+    <col min="1" max="1" width="33.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="3.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="37.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="37.5703125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="27.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -1382,7 +1382,7 @@
       </c>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>10</v>
       </c>
@@ -1402,7 +1402,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>242</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>198</v>
       </c>
@@ -1442,11 +1442,11 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
-        <v>278</v>
-      </c>
-      <c r="B5" s="4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="D5" s="7" t="s">
@@ -1462,7 +1462,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -1482,7 +1482,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -1502,7 +1502,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>153</v>
       </c>
@@ -1542,7 +1542,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>213</v>
       </c>
@@ -1562,7 +1562,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>18</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>20</v>
       </c>
@@ -1602,7 +1602,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1622,7 +1622,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>23</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
         <v>277</v>
       </c>
@@ -1662,7 +1662,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="3" t="s">
         <v>62</v>
       </c>
@@ -1676,7 +1676,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
         <v>126</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>132</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>131</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>130</v>
       </c>
@@ -1754,7 +1754,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
         <v>57</v>
       </c>
@@ -1768,7 +1768,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
         <v>28</v>
       </c>
@@ -1786,7 +1786,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>228</v>
       </c>
@@ -1800,13 +1800,13 @@
         <v>267</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>167</v>
       </c>
@@ -1826,7 +1826,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>29</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>229</v>
       </c>
@@ -1866,7 +1866,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>164</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>212</v>
       </c>
@@ -1906,7 +1906,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>32</v>
       </c>
@@ -1926,7 +1926,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
         <v>50</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="14" t="s">
         <v>70</v>
       </c>
@@ -1958,7 +1958,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>176</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>80</v>
       </c>
@@ -1998,7 +1998,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>6</v>
       </c>
@@ -2018,7 +2018,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>81</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>82</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>83</v>
       </c>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>84</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>85</v>
       </c>
@@ -2110,7 +2110,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>86</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>88</v>
       </c>
@@ -2170,7 +2170,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>175</v>
       </c>
@@ -2190,7 +2190,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D44" s="3" t="s">
         <v>159</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="13" t="s">
         <v>133</v>
       </c>
@@ -2214,7 +2214,7 @@
       </c>
       <c r="H45" s="13"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>183</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>135</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>275</v>
       </c>
@@ -2274,7 +2274,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>157</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>174</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>185</v>
       </c>

</xml_diff>

<commit_message>
IntelliJ Shortcuts table layout
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1349,10 +1349,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A16" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2294,7 +2294,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>174</v>
       </c>
@@ -2314,24 +2314,26 @@
         <v>207</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>185</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>186</v>
       </c>
-      <c r="D51" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="20" t="s">
-        <v>220</v>
-      </c>
       <c r="G51" s="5" t="s">
         <v>216</v>
       </c>
       <c r="H51" s="6" t="s">
         <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D52" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="20" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Live Templates to IntelliJ Shortcuts
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Wiki\Settings\IntelliJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E956F7E5-D75F-4964-88A3-4D88491E56A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218E49F6-7575-436D-91EE-BD581E0B33F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="323">
   <si>
     <t>Smart code completion</t>
   </si>
@@ -917,6 +917,93 @@
   </si>
   <si>
     <t>Get from Version Control</t>
+  </si>
+  <si>
+    <t>sout</t>
+  </si>
+  <si>
+    <t>soutm</t>
+  </si>
+  <si>
+    <t>soutp</t>
+  </si>
+  <si>
+    <t>soutv</t>
+  </si>
+  <si>
+    <t>souf</t>
+  </si>
+  <si>
+    <t>public static void main</t>
+  </si>
+  <si>
+    <t>System.out</t>
+  </si>
+  <si>
+    <t>System.out method name</t>
+  </si>
+  <si>
+    <t>System.out paramaters</t>
+  </si>
+  <si>
+    <t>System.out value</t>
+  </si>
+  <si>
+    <t>System.out.printf</t>
+  </si>
+  <si>
+    <t>iter</t>
+  </si>
+  <si>
+    <t>itco</t>
+  </si>
+  <si>
+    <t>itar</t>
+  </si>
+  <si>
+    <t>Iterator</t>
+  </si>
+  <si>
+    <t>Iterate collection</t>
+  </si>
+  <si>
+    <t>Iterate array</t>
+  </si>
+  <si>
+    <t>itli</t>
+  </si>
+  <si>
+    <t>Iterate list</t>
+  </si>
+  <si>
+    <t>fori</t>
+  </si>
+  <si>
+    <t>for loop</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>Surround with method call</t>
+  </si>
+  <si>
+    <t>psvm / main</t>
+  </si>
+  <si>
+    <t>psf</t>
+  </si>
+  <si>
+    <t>prsf</t>
+  </si>
+  <si>
+    <t>public static final</t>
+  </si>
+  <si>
+    <t>private static final</t>
+  </si>
+  <si>
+    <t>Live Templates</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1073,6 +1160,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1416,10 +1508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A25" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1432,10 +1524,12 @@
     <col min="6" max="6" width="3.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="37.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.42578125" style="2"/>
+    <col min="9" max="9" width="11.42578125" style="2"/>
+    <col min="10" max="10" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1448,8 +1542,12 @@
         <v>86</v>
       </c>
       <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="25" t="s">
+        <v>322</v>
+      </c>
+      <c r="J1" s="25"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -1468,8 +1566,14 @@
       <c r="H2" s="4" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="J2" s="23" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>283</v>
       </c>
@@ -1488,8 +1592,14 @@
       <c r="H3" s="4" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="J3" s="24" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>190</v>
       </c>
@@ -1508,8 +1618,14 @@
       <c r="H4" s="4" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="J4" s="23" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>266</v>
       </c>
@@ -1528,8 +1644,14 @@
       <c r="H5" s="4" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="24" t="s">
+        <v>297</v>
+      </c>
+      <c r="J5" s="24" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1548,8 +1670,14 @@
       <c r="H6" s="4" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I6" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="J6" s="24" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -1569,7 +1697,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -1588,8 +1716,14 @@
       <c r="H8" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I8" s="24" t="s">
+        <v>317</v>
+      </c>
+      <c r="J8" s="24" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>148</v>
       </c>
@@ -1608,8 +1742,14 @@
       <c r="H9" s="8" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>205</v>
       </c>
@@ -1628,8 +1768,14 @@
       <c r="H10" s="4" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I10" s="24" t="s">
+        <v>319</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>16</v>
       </c>
@@ -1649,7 +1795,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>285</v>
       </c>
@@ -1668,8 +1814,14 @@
       <c r="H12" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="23" t="s">
+        <v>305</v>
+      </c>
+      <c r="J12" s="23" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -1688,8 +1840,14 @@
       <c r="H13" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I13" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
@@ -1708,8 +1866,14 @@
       <c r="H14" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I14" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>263</v>
       </c>
@@ -1728,8 +1892,14 @@
       <c r="H15" s="4" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I15" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="J15" s="24" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>287</v>
       </c>
@@ -1748,8 +1918,14 @@
       <c r="H16" s="4" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I16" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="J16" s="24" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>123</v>
       </c>
@@ -1767,7 +1943,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>129</v>
       </c>
@@ -1786,8 +1962,14 @@
       <c r="H18" s="4" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I18" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>128</v>
       </c>
@@ -1807,7 +1989,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>127</v>
       </c>
@@ -1827,7 +2009,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
         <v>55</v>
       </c>
@@ -1841,7 +2023,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>25</v>
       </c>
@@ -1859,7 +2041,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>217</v>
       </c>
@@ -1879,7 +2061,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>162</v>
       </c>
@@ -1899,7 +2081,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>26</v>
       </c>
@@ -1919,7 +2101,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>218</v>
       </c>
@@ -1939,7 +2121,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>159</v>
       </c>
@@ -1959,7 +2141,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>204</v>
       </c>
@@ -1979,7 +2161,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>29</v>
       </c>
@@ -1999,7 +2181,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
         <v>48</v>
       </c>
@@ -2013,7 +2195,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
         <v>67</v>
       </c>
@@ -2031,7 +2213,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>171</v>
       </c>
@@ -2440,6 +2622,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
   <headerFooter>

</xml_diff>

<commit_message>
learn IntelliJ with Heinz Kabutz
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218E49F6-7575-436D-91EE-BD581E0B33F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A4D3CA-0046-469C-AB0F-EFC397BA2FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>Alt + Enter</t>
   </si>
   <si>
-    <t>Ctrl + P</t>
-  </si>
-  <si>
     <t>Rename</t>
   </si>
   <si>
@@ -538,9 +535,6 @@
     <t>Move Element Left/Right</t>
   </si>
   <si>
-    <t>Copy / Move</t>
-  </si>
-  <si>
     <t>F5 / F6</t>
   </si>
   <si>
@@ -668,9 +662,6 @@
   </si>
   <si>
     <t>Ctrl + Shift + F9/10</t>
-  </si>
-  <si>
-    <t>Parameter info (within method call args)</t>
   </si>
   <si>
     <t>Double Shift / Ctrl + Shift + A</t>
@@ -1004,6 +995,15 @@
   </si>
   <si>
     <t>Live Templates</t>
+  </si>
+  <si>
+    <t>Copy / Move (Class, Method, Field)</t>
+  </si>
+  <si>
+    <t>Parameter info (in method call args) / Type info</t>
+  </si>
+  <si>
+    <t>Ctrl + P / Ctrl + Shift + P</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1130,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1165,6 +1165,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1511,7 +1513,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,54 +1533,54 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1"/>
       <c r="D1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E1" s="1"/>
       <c r="G1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="25" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J1" s="25"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>9</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>0</v>
@@ -1587,76 +1589,76 @@
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>2</v>
@@ -1665,960 +1667,960 @@
         <v>3</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>215</v>
+      <c r="D7" s="27" t="s">
+        <v>321</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>4</v>
+        <v>322</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>15</v>
-      </c>
       <c r="D8" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>17</v>
-      </c>
       <c r="D11" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I12" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="J12" s="23" t="s">
         <v>305</v>
-      </c>
-      <c r="J12" s="23" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>19</v>
-      </c>
       <c r="D13" s="7" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I13" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="J13" s="24" t="s">
         <v>306</v>
-      </c>
-      <c r="J13" s="24" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I14" s="24" t="s">
+        <v>304</v>
+      </c>
+      <c r="J14" s="24" t="s">
         <v>307</v>
-      </c>
-      <c r="J14" s="24" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B17" s="11"/>
       <c r="D17" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E17" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E18" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="G17" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>132</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="E19" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>144</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="11"/>
       <c r="D22" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>27</v>
-      </c>
       <c r="D25" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>160</v>
-      </c>
       <c r="D27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>158</v>
-      </c>
       <c r="G29" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H29" s="4" t="s">
         <v>103</v>
-      </c>
-      <c r="H29" s="4" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="12"/>
       <c r="D31" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>171</v>
+      <c r="A32" s="26" t="s">
+        <v>320</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="E33" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="G33" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="G33" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="H33" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B34" s="8" t="s">
-        <v>6</v>
-      </c>
       <c r="D34" s="3" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="G34" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="H34" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="H34" s="4" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="G38" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="H39" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D44" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="E44" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E44" s="4" t="s">
-        <v>156</v>
-      </c>
       <c r="G44" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B45" s="11"/>
       <c r="D45" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G45" s="17" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D46" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E46" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="E46" s="4" t="s">
-        <v>168</v>
-      </c>
       <c r="G46" s="5" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G47" s="11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H47" s="20"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="G51" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H51" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="H51" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update IntelliJ plugins and shortcuts
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36A4D3CA-0046-469C-AB0F-EFC397BA2FE0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C608238B-FE1E-40C4-9BFF-BD4AEF526273}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="334">
   <si>
     <t>Smart code completion</t>
   </si>
@@ -1004,6 +1004,59 @@
   </si>
   <si>
     <t>Ctrl + P / Ctrl + Shift + P</t>
+  </si>
+  <si>
+    <t>Inspections</t>
+  </si>
+  <si>
+    <t>Code style issues &gt; Field may be 'final'</t>
+  </si>
+  <si>
+    <t>Declaration redundancy &gt; Unused declaration</t>
+  </si>
+  <si>
+    <t>Run Inspection by Name</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + Shift + I</t>
+  </si>
+  <si>
+    <t>Select specific inspections</t>
+  </si>
+  <si>
+    <t>Analyze &gt; Inspect Code &gt; Inspection profile &gt; …</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Recommended </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Inspections &gt; Java</t>
+    </r>
+  </si>
+  <si>
+    <t>Error handling</t>
+  </si>
+  <si>
+    <t>Code maturity</t>
+  </si>
+  <si>
+    <t>Java language level migration aids</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1162,11 +1215,13 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1513,7 +1568,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1526,8 +1581,8 @@
     <col min="6" max="6" width="3.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="37.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" style="2"/>
-    <col min="10" max="10" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="43" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -1544,10 +1599,10 @@
         <v>85</v>
       </c>
       <c r="H1" s="1"/>
-      <c r="I1" s="25" t="s">
+      <c r="I1" s="27" t="s">
         <v>319</v>
       </c>
-      <c r="J1" s="25"/>
+      <c r="J1" s="27"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1686,7 +1741,7 @@
       <c r="B7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D7" s="27" t="s">
+      <c r="D7" s="26" t="s">
         <v>321</v>
       </c>
       <c r="E7" s="8" t="s">
@@ -2010,6 +2065,10 @@
       <c r="H20" s="4" t="s">
         <v>194</v>
       </c>
+      <c r="I20" s="27" t="s">
+        <v>323</v>
+      </c>
+      <c r="J20" s="27"/>
     </row>
     <row r="21" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D21" s="3" t="s">
@@ -2024,6 +2083,12 @@
       <c r="H21" s="4" t="s">
         <v>97</v>
       </c>
+      <c r="I21" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="J21" s="29" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="22" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
@@ -2042,6 +2107,12 @@
       <c r="H22" s="4" t="s">
         <v>98</v>
       </c>
+      <c r="I22" s="24" t="s">
+        <v>328</v>
+      </c>
+      <c r="J22" s="28" t="s">
+        <v>329</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -2082,6 +2153,9 @@
       <c r="H24" s="4" t="s">
         <v>99</v>
       </c>
+      <c r="I24" s="28" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="25" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
@@ -2102,6 +2176,9 @@
       <c r="H25" s="4" t="s">
         <v>100</v>
       </c>
+      <c r="I25" s="24" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="26" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
@@ -2122,6 +2199,9 @@
       <c r="H26" s="4" t="s">
         <v>101</v>
       </c>
+      <c r="I26" s="24" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
@@ -2142,6 +2222,9 @@
       <c r="H27" s="4" t="s">
         <v>186</v>
       </c>
+      <c r="I27" s="24" t="s">
+        <v>332</v>
+      </c>
     </row>
     <row r="28" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
@@ -2162,6 +2245,9 @@
       <c r="H28" s="4" t="s">
         <v>229</v>
       </c>
+      <c r="I28" s="24" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="29" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
@@ -2182,6 +2268,9 @@
       <c r="H29" s="4" t="s">
         <v>103</v>
       </c>
+      <c r="I29" s="24" t="s">
+        <v>333</v>
+      </c>
     </row>
     <row r="30" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="3" t="s">
@@ -2216,7 +2305,7 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="26" t="s">
+      <c r="A32" s="25" t="s">
         <v>320</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -2624,8 +2713,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="I1:J1"/>
+    <mergeCell ref="I20:J20"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
navigate symbols in IntelliJ
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5202390-1D15-4583-BA71-815E4D8BCE97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD29191-78F5-4747-93A4-7A628D475B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -286,12 +286,6 @@
     <t>Ctrl + Alt + Shift + N</t>
   </si>
   <si>
-    <t>F12</t>
-  </si>
-  <si>
-    <t>Esc</t>
-  </si>
-  <si>
     <t>Shift + Esc</t>
   </si>
   <si>
@@ -356,12 +350,6 @@
   </si>
   <si>
     <t>Go to symbol</t>
-  </si>
-  <si>
-    <t>Go back to previous tool window</t>
-  </si>
-  <si>
-    <t>Go to editor (from tool window)</t>
   </si>
   <si>
     <t>Hide active or last active window</t>
@@ -866,9 +854,6 @@
   </si>
   <si>
     <t>Next/Previous Project Window</t>
-  </si>
-  <si>
-    <t>Ctrl + Alt + +/ü</t>
   </si>
   <si>
     <t>Quick List "Tool Windows"</t>
@@ -1063,6 +1048,21 @@
   </si>
   <si>
     <t>Search everywhere / …more</t>
+  </si>
+  <si>
+    <t>Focus Editor / Jump to Last Tool Window</t>
+  </si>
+  <si>
+    <t>Esc / F12</t>
+  </si>
+  <si>
+    <t>Go to next / prev highl. element usage</t>
+  </si>
+  <si>
+    <t>Ctrl + , / Ctrl + Shift + ,</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + +/Ü</t>
   </si>
 </sst>
 </file>
@@ -1574,7 +1574,7 @@
   <dimension ref="A1:J52"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="29" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="J1" s="29"/>
     </row>
@@ -1624,24 +1624,24 @@
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>0</v>
@@ -1650,24 +1650,24 @@
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>86</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>64</v>
@@ -1676,42 +1676,42 @@
         <v>31</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>111</v>
+        <v>270</v>
+      </c>
+      <c r="G5" s="25" t="s">
+        <v>331</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>87</v>
+        <v>332</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -1728,16 +1728,16 @@
         <v>3</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1748,16 +1748,16 @@
         <v>12</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1773,25 +1773,25 @@
       <c r="E8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>90</v>
+      <c r="G8" s="21" t="s">
+        <v>281</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>282</v>
       </c>
       <c r="I8" s="24" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>56</v>
@@ -1799,43 +1799,43 @@
       <c r="E9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G9" s="21" t="s">
-        <v>286</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>287</v>
+      <c r="G9" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>215</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>244</v>
+        <v>111</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>219</v>
+        <v>89</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1849,21 +1849,21 @@
         <v>62</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>61</v>
@@ -1872,16 +1872,16 @@
         <v>33</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>116</v>
+        <v>248</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>92</v>
+        <v>244</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -1898,16 +1898,16 @@
         <v>34</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>252</v>
+        <v>113</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>248</v>
+        <v>91</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -1918,30 +1918,30 @@
         <v>20</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>59</v>
@@ -1950,114 +1950,114 @@
         <v>35</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>108</v>
+        <v>239</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="J16" s="24" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B17" s="11"/>
       <c r="D17" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>96</v>
+        <v>216</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>128</v>
+      <c r="A18" s="25" t="s">
+        <v>124</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>57</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>220</v>
+        <v>127</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>176</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>178</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="H19" s="6" t="s">
-        <v>180</v>
+        <v>174</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>55</v>
@@ -2066,13 +2066,13 @@
         <v>37</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>194</v>
+        <v>95</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="J20" s="29"/>
     </row>
@@ -2087,24 +2087,24 @@
         <v>38</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="J21" s="28" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>53</v>
@@ -2112,25 +2112,25 @@
       <c r="E22" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="G22" s="3" t="s">
-        <v>106</v>
+      <c r="G22" s="14" t="s">
+        <v>256</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>98</v>
+        <v>255</v>
       </c>
       <c r="I22" s="24" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="J22" s="27" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>52</v>
@@ -2138,34 +2138,34 @@
       <c r="E23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="G23" s="14" t="s">
-        <v>260</v>
+      <c r="G23" s="3" t="s">
+        <v>103</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>259</v>
+        <v>97</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>105</v>
+        <v>181</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2179,47 +2179,47 @@
         <v>50</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>185</v>
+        <v>102</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>104</v>
+        <v>183</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>101</v>
+        <v>182</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>48</v>
@@ -2228,36 +2228,36 @@
         <v>41</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>226</v>
+        <v>100</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>227</v>
+        <v>101</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2268,33 +2268,39 @@
         <v>27</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>102</v>
+        <v>134</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>103</v>
+        <v>263</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>334</v>
+      </c>
       <c r="D30" s="3" t="s">
         <v>47</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="H30" s="4" t="s">
-        <v>267</v>
+      <c r="G30" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2308,31 +2314,31 @@
       <c r="E31" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>268</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>269</v>
+      <c r="G31" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="25" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>139</v>
+        <v>237</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>224</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2343,13 +2349,13 @@
         <v>75</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>241</v>
+        <v>132</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>133</v>
@@ -2363,16 +2369,16 @@
         <v>5</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>136</v>
+        <v>179</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>137</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2383,16 +2389,16 @@
         <v>74</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>233</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="H35" s="4" t="s">
-        <v>184</v>
+        <v>229</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2408,11 +2414,11 @@
       <c r="E36" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G36" s="13" t="s">
-        <v>253</v>
+      <c r="G36" s="5" t="s">
+        <v>272</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>231</v>
+        <v>335</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2423,17 +2429,15 @@
         <v>72</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>276</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>277</v>
-      </c>
+        <v>251</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H37" s="1"/>
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
@@ -2443,15 +2447,17 @@
         <v>71</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="H38" s="1"/>
+        <v>131</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
@@ -2461,16 +2467,16 @@
         <v>70</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G39" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="H39" s="4" t="s">
-        <v>119</v>
+      <c r="G39" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2481,16 +2487,16 @@
         <v>69</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>208</v>
+        <v>141</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2501,16 +2507,16 @@
         <v>68</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>221</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H41" s="4" t="s">
-        <v>210</v>
+        <v>217</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2521,102 +2527,96 @@
         <v>67</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>222</v>
-      </c>
-      <c r="G42" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>212</v>
+        <v>218</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>240</v>
+        <v>195</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D44" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="G44" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="H44" s="4" t="s">
-        <v>200</v>
+        <v>151</v>
+      </c>
+      <c r="G44" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="H44" s="18" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B45" s="11"/>
       <c r="D45" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="G45" s="17" t="s">
-        <v>270</v>
-      </c>
-      <c r="H45" s="18" t="s">
-        <v>271</v>
+        <v>148</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>279</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>285</v>
+        <v>163</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G47" s="11" t="s">
         <v>21</v>
@@ -2625,76 +2625,76 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H48" s="4" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H49" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="E51" s="16" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>22</v>
@@ -2705,22 +2705,22 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add EN shortcuts for IntelliJ
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCD29191-78F5-4747-93A4-7A628D475B25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE3DEC7-1A47-4F8F-B027-D736D59A9A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="347">
   <si>
     <t>Smart code completion</t>
   </si>
@@ -854,9 +854,6 @@
   </si>
   <si>
     <t>Next/Previous Project Window</t>
-  </si>
-  <si>
-    <t>Quick List "Tool Windows"</t>
   </si>
   <si>
     <t>Ctrl + Shift + Circumflex (^)</t>
@@ -1064,12 +1061,48 @@
   <si>
     <t>Ctrl + Alt + +/Ü</t>
   </si>
+  <si>
+    <t>Ctrl + Shift + `</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + '</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + '</t>
+  </si>
+  <si>
+    <t>Ctrl + `</t>
+  </si>
+  <si>
+    <t>Branches</t>
+  </si>
+  <si>
+    <t>Alt + `</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt + [/]</t>
+  </si>
+  <si>
+    <t>Previous/next Project Window</t>
+  </si>
+  <si>
+    <t>Ctrl + [/]</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + [/]</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + ;</t>
+  </si>
+  <si>
+    <t>Ctrl + \ / Ctrl + Shift + \</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1106,8 +1139,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1130,6 +1170,11 @@
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59996337778862885"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1186,10 +1231,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1228,8 +1274,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1571,10 +1619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:J104"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A60" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,7 +1654,7 @@
       </c>
       <c r="H1" s="1"/>
       <c r="I1" s="29" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="J1" s="29"/>
     </row>
@@ -1630,18 +1678,18 @@
         <v>200</v>
       </c>
       <c r="I2" s="23" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J2" s="23" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>273</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>274</v>
+      <c r="A3" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>158</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>0</v>
@@ -1656,18 +1704,18 @@
         <v>86</v>
       </c>
       <c r="I3" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>158</v>
+      <c r="A4" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>64</v>
@@ -1682,18 +1730,18 @@
         <v>214</v>
       </c>
       <c r="I4" s="23" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J4" s="23" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>276</v>
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>271</v>
@@ -1702,24 +1750,24 @@
         <v>270</v>
       </c>
       <c r="G5" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>332</v>
-      </c>
       <c r="I5" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>2</v>
@@ -1734,24 +1782,24 @@
         <v>87</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>314</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>315</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>110</v>
@@ -1761,11 +1809,11 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>14</v>
+      <c r="A8" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>177</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>63</v>
@@ -1774,24 +1822,24 @@
         <v>32</v>
       </c>
       <c r="G8" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="H8" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="H8" s="8" t="s">
-        <v>282</v>
-      </c>
       <c r="I8" s="24" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="J8" s="24" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>177</v>
+      <c r="A9" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>211</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>56</v>
@@ -1806,18 +1854,18 @@
         <v>215</v>
       </c>
       <c r="I9" s="24" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="J9" s="24" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>211</v>
+      <c r="A10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>145</v>
@@ -1832,18 +1880,18 @@
         <v>89</v>
       </c>
       <c r="I10" s="24" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="J10" s="24" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>16</v>
+      <c r="A11" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>62</v>
@@ -1859,11 +1907,11 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
-        <v>275</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>137</v>
+      <c r="A12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>61</v>
@@ -1878,18 +1926,18 @@
         <v>244</v>
       </c>
       <c r="I12" s="23" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J12" s="23" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>60</v>
@@ -1904,18 +1952,18 @@
         <v>91</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
+      <c r="A14" s="14" t="s">
+        <v>254</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>253</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>168</v>
@@ -1930,18 +1978,18 @@
         <v>92</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J14" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>59</v>
@@ -1956,19 +2004,17 @@
         <v>93</v>
       </c>
       <c r="I15" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="J15" s="24" t="s">
         <v>301</v>
       </c>
-      <c r="J15" s="24" t="s">
-        <v>302</v>
-      </c>
     </row>
     <row r="16" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>277</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>278</v>
-      </c>
+      <c r="A16" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B16" s="11"/>
       <c r="D16" s="3" t="s">
         <v>170</v>
       </c>
@@ -1982,17 +2028,19 @@
         <v>94</v>
       </c>
       <c r="I16" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="J16" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="J16" s="24" t="s">
-        <v>304</v>
-      </c>
     </row>
     <row r="17" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B17" s="11"/>
+      <c r="A17" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D17" s="3" t="s">
         <v>58</v>
       </c>
@@ -2007,11 +2055,11 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25" t="s">
-        <v>124</v>
+      <c r="A18" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>57</v>
@@ -2026,18 +2074,18 @@
         <v>176</v>
       </c>
       <c r="I18" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J18" s="5" t="s">
         <v>305</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>306</v>
-      </c>
     </row>
     <row r="19" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>120</v>
+      <c r="A19" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="D19" s="7" t="s">
         <v>221</v>
@@ -2053,11 +2101,8 @@
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>121</v>
+      <c r="A20" s="11" t="s">
+        <v>24</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>55</v>
@@ -2072,13 +2117,16 @@
         <v>95</v>
       </c>
       <c r="I20" s="29" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="J20" s="29"/>
     </row>
     <row r="21" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="11" t="s">
-        <v>24</v>
+      <c r="A21" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>328</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>54</v>
@@ -2093,18 +2141,18 @@
         <v>96</v>
       </c>
       <c r="I21" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="J21" s="28" t="s">
         <v>319</v>
-      </c>
-      <c r="J21" s="28" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>53</v>
@@ -2119,18 +2167,18 @@
         <v>255</v>
       </c>
       <c r="I22" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="J22" s="27" t="s">
         <v>321</v>
       </c>
-      <c r="J22" s="27" t="s">
-        <v>322</v>
-      </c>
     </row>
     <row r="23" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
-        <v>327</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>328</v>
+      <c r="A23" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>52</v>
@@ -2147,10 +2195,10 @@
     </row>
     <row r="24" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>157</v>
+        <v>25</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>51</v>
@@ -2165,15 +2213,15 @@
         <v>98</v>
       </c>
       <c r="I24" s="27" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>25</v>
+        <v>209</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>50</v>
@@ -2188,15 +2236,15 @@
         <v>99</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>209</v>
+        <v>154</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>210</v>
+        <v>155</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>49</v>
@@ -2211,15 +2259,15 @@
         <v>182</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>48</v>
@@ -2234,15 +2282,15 @@
         <v>223</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>198</v>
+        <v>28</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>197</v>
+        <v>27</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>224</v>
@@ -2257,16 +2305,14 @@
         <v>101</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="A29" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B29" s="30"/>
       <c r="D29" s="3" t="s">
         <v>152</v>
       </c>
@@ -2280,16 +2326,14 @@
         <v>263</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="22" t="s">
-        <v>333</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>334</v>
-      </c>
+      <c r="A30" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B30" s="12"/>
       <c r="D30" s="3" t="s">
         <v>47</v>
       </c>
@@ -2304,10 +2348,12 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="12"/>
+      <c r="A31" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>166</v>
+      </c>
       <c r="D31" s="3" t="s">
         <v>46</v>
       </c>
@@ -2322,11 +2368,11 @@
       </c>
     </row>
     <row r="32" spans="1:10" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="25" t="s">
-        <v>313</v>
+      <c r="A32" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>166</v>
+        <v>75</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>232</v>
@@ -2342,11 +2388,11 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>75</v>
+      <c r="A33" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>233</v>
@@ -2362,11 +2408,11 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>5</v>
+      <c r="A34" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>74</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>231</v>
@@ -2383,10 +2429,10 @@
     </row>
     <row r="35" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>230</v>
@@ -2403,10 +2449,10 @@
     </row>
     <row r="36" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>45</v>
@@ -2418,15 +2464,15 @@
         <v>272</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D37" s="5" t="s">
         <v>250</v>
@@ -2441,10 +2487,10 @@
     </row>
     <row r="38" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D38" s="5" t="s">
         <v>130</v>
@@ -2461,10 +2507,10 @@
     </row>
     <row r="39" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>140</v>
@@ -2481,10 +2527,10 @@
     </row>
     <row r="40" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>142</v>
@@ -2501,10 +2547,10 @@
     </row>
     <row r="41" spans="1:8" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D41" s="3" t="s">
         <v>128</v>
@@ -2521,10 +2567,10 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>67</v>
+        <v>212</v>
       </c>
       <c r="D42" s="3" t="s">
         <v>136</v>
@@ -2540,12 +2586,6 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>212</v>
-      </c>
       <c r="D43" s="3" t="s">
         <v>242</v>
       </c>
@@ -2560,6 +2600,10 @@
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" s="11"/>
       <c r="D44" s="3" t="s">
         <v>150</v>
       </c>
@@ -2574,10 +2618,12 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B45" s="11"/>
+      <c r="A45" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>173</v>
+      </c>
       <c r="D45" s="3" t="s">
         <v>149</v>
       </c>
@@ -2585,18 +2631,18 @@
         <v>148</v>
       </c>
       <c r="G45" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="H45" s="6" t="s">
         <v>279</v>
       </c>
-      <c r="H45" s="6" t="s">
-        <v>280</v>
-      </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>172</v>
+      <c r="A46" s="14" t="s">
+        <v>258</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>173</v>
+        <v>259</v>
       </c>
       <c r="D46" s="3" t="s">
         <v>162</v>
@@ -2606,11 +2652,11 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>259</v>
+      <c r="A47" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B47" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="D47" s="3" t="s">
         <v>160</v>
@@ -2624,11 +2670,11 @@
       <c r="H47" s="20"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>252</v>
+      <c r="A48" s="19" t="s">
+        <v>339</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>138</v>
+        <v>273</v>
       </c>
       <c r="D48" s="3" t="s">
         <v>149</v>
@@ -2705,7 +2751,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>260</v>
@@ -2720,6 +2766,1015 @@
         <v>194</v>
       </c>
       <c r="H52" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B53" s="1"/>
+      <c r="D53" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="1"/>
+      <c r="G53" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H53" s="1"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="H54" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H55" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="H56" s="4" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="G57" s="25" t="s">
+        <v>330</v>
+      </c>
+      <c r="H57" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H58" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D59" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H59" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G60" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="H60" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H61" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E62" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H62" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="14" t="s">
+        <v>274</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>338</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H63" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="H64" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E65" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="H65" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H66" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="14" t="s">
+        <v>276</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H67" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" s="11"/>
+      <c r="D68" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="H68" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="H69" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="G70" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="H70" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D71" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E71" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="H71" s="4" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H72" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="H73" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="26" t="s">
+        <v>326</v>
+      </c>
+      <c r="B74" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G74" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="H74" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="H75" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="H76" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="H77" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="H78" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H79" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="H80" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="H81" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82" s="12"/>
+      <c r="D82" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H82" s="6" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H83" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>344</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H84" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B85" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H85" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H86" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="G87" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="H87" s="6" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="H88" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B89" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D89" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H89" s="1"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D90" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E90" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H90" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B91" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E91" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G91" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H91" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B92" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E92" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G92" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H92" s="4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B93" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="G93" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H93" s="6" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="B94" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E94" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H94" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D95" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H95" s="4" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B96" s="11"/>
+      <c r="D96" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G96" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="H96" s="18" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="G97" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="H97" s="6" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" s="14" t="s">
+        <v>258</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="G99" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H99" s="20"/>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" s="25" t="s">
+        <v>339</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H100" s="4" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H101" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="D102" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E102" s="16" t="s">
+        <v>346</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="D103" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E103" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H103" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" s="22" t="s">
+        <v>282</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="D104" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E104" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="H104" s="4" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Shortut and WinTerm update
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D48D15-37B2-4242-AE9C-F54D3F522B63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9F9328-4E21-4E40-91FD-75E33086A4A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1241,7 +1241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1284,6 +1284,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -1630,18 +1634,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J113"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A37" zoomScale="115" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A76" zoomScale="115" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" style="2" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="3.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2.28515625" style="2" customWidth="1"/>
     <col min="4" max="4" width="41.140625" style="2" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="2.28515625" style="2" customWidth="1"/>
     <col min="7" max="7" width="37.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="22.5703125" style="2" customWidth="1"/>
@@ -1659,12 +1663,39 @@
       </c>
       <c r="J1" s="30"/>
     </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
     <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1"/>
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>200</v>
+      </c>
       <c r="I3" s="31" t="s">
         <v>311</v>
       </c>
@@ -1672,19 +1703,23 @@
     </row>
     <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>184</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H4" s="1"/>
+        <v>158</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="I4" s="23" t="s">
         <v>283</v>
       </c>
@@ -1693,23 +1728,23 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>158</v>
+      <c r="A5" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>200</v>
+        <v>214</v>
       </c>
       <c r="I5" s="24" t="s">
         <v>284</v>
@@ -1719,23 +1754,23 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>257</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>108</v>
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>271</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>330</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>86</v>
+        <v>331</v>
       </c>
       <c r="I6" s="23" t="s">
         <v>285</v>
@@ -1746,22 +1781,22 @@
     </row>
     <row r="7" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>31</v>
+        <v>12</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>3</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>241</v>
+        <v>109</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>214</v>
+        <v>87</v>
       </c>
       <c r="I7" s="24" t="s">
         <v>286</v>
@@ -1772,22 +1807,22 @@
     </row>
     <row r="8" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>271</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>330</v>
+        <v>14</v>
+      </c>
+      <c r="D8" s="26" t="s">
+        <v>313</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>331</v>
+        <v>88</v>
       </c>
       <c r="I8" s="24" t="s">
         <v>287</v>
@@ -1797,43 +1832,43 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>87</v>
+      <c r="A9" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="D10" s="26" t="s">
-        <v>313</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>314</v>
+      <c r="A10" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>110</v>
+        <v>240</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>88</v>
+        <v>215</v>
       </c>
       <c r="I10" s="24" t="s">
         <v>306</v>
@@ -1843,23 +1878,23 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>211</v>
+      <c r="A11" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>63</v>
+        <v>145</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="21" t="s">
-        <v>280</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>281</v>
+        <v>144</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>89</v>
       </c>
       <c r="I11" s="24" t="s">
         <v>307</v>
@@ -1869,23 +1904,23 @@
       </c>
     </row>
     <row r="12" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>16</v>
+      <c r="A12" s="19" t="s">
+        <v>274</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>36</v>
+        <v>178</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>240</v>
+        <v>112</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>215</v>
+        <v>90</v>
       </c>
       <c r="I12" s="24" t="s">
         <v>308</v>
@@ -1895,43 +1930,43 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
-        <v>274</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>137</v>
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>145</v>
+        <v>61</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>144</v>
+        <v>33</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>111</v>
+        <v>248</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>89</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>178</v>
+        <v>20</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I14" s="23" t="s">
         <v>294</v>
@@ -1941,23 +1976,23 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>19</v>
+      <c r="A15" s="14" t="s">
+        <v>254</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>20</v>
+        <v>253</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>61</v>
+        <v>168</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>33</v>
+        <v>169</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>248</v>
+        <v>107</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>244</v>
+        <v>92</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>295</v>
@@ -1968,22 +2003,22 @@
     </row>
     <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>254</v>
+        <v>276</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>34</v>
+        <v>277</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>35</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="I16" s="24" t="s">
         <v>296</v>
@@ -1993,23 +2028,17 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>277</v>
-      </c>
       <c r="D17" s="3" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>107</v>
+        <v>239</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I17" s="24" t="s">
         <v>300</v>
@@ -2019,17 +2048,21 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="11"/>
       <c r="D18" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>35</v>
+        <v>126</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>106</v>
+        <v>238</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>93</v>
+        <v>216</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>302</v>
@@ -2039,41 +2072,43 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B19" s="11"/>
+      <c r="A19" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D19" s="3" t="s">
-        <v>170</v>
+        <v>57</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>239</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>94</v>
+        <v>127</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="25" t="s">
-        <v>124</v>
+      <c r="A20" s="3" t="s">
+        <v>123</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>126</v>
+        <v>120</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>174</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>238</v>
+        <v>189</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="I20" s="5" t="s">
         <v>304</v>
@@ -2083,43 +2118,37 @@
       </c>
     </row>
     <row r="21" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>120</v>
+      <c r="A21" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>121</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>176</v>
+        <v>37</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>221</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>174</v>
+      <c r="D22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>189</v>
+        <v>104</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>190</v>
+        <v>96</v>
       </c>
       <c r="I22" s="31" t="s">
         <v>315</v>
@@ -2127,17 +2156,20 @@
       <c r="J22" s="31"/>
     </row>
     <row r="23" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="D23" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>105</v>
+        <v>39</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>256</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>95</v>
+        <v>255</v>
       </c>
       <c r="I23" s="24" t="s">
         <v>318</v>
@@ -2147,20 +2179,23 @@
       </c>
     </row>
     <row r="24" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11" t="s">
-        <v>24</v>
+      <c r="A24" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>328</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="I24" s="24" t="s">
         <v>320</v>
@@ -2171,42 +2206,42 @@
     </row>
     <row r="25" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>256</v>
+        <v>245</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>181</v>
       </c>
       <c r="H25" s="4" t="s">
-        <v>255</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>326</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>327</v>
+      <c r="A26" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>156</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>40</v>
+        <v>247</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="I26" s="27" t="s">
         <v>322</v>
@@ -2214,22 +2249,22 @@
     </row>
     <row r="27" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>157</v>
+        <v>25</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>156</v>
+        <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>98</v>
+        <v>182</v>
       </c>
       <c r="I27" s="24" t="s">
         <v>316</v>
@@ -2237,22 +2272,22 @@
     </row>
     <row r="28" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>209</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>26</v>
+        <v>210</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>247</v>
+        <v>41</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>102</v>
+        <v>222</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>99</v>
+        <v>223</v>
       </c>
       <c r="I28" s="24" t="s">
         <v>317</v>
@@ -2260,22 +2295,22 @@
     </row>
     <row r="29" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>209</v>
+        <v>154</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>210</v>
+        <v>155</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>49</v>
+        <v>224</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>246</v>
+        <v>225</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>183</v>
+        <v>100</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>182</v>
+        <v>101</v>
       </c>
       <c r="I29" s="24" t="s">
         <v>324</v>
@@ -2283,22 +2318,22 @@
     </row>
     <row r="30" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>197</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>41</v>
+        <v>153</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>222</v>
+        <v>134</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="I30" s="24" t="s">
         <v>323</v>
@@ -2306,499 +2341,468 @@
     </row>
     <row r="31" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>198</v>
+        <v>28</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>197</v>
+        <v>27</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>224</v>
+        <v>47</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H31" s="4" t="s">
-        <v>101</v>
+        <v>42</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="I31" s="24" t="s">
         <v>325</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="A32" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="B32" s="29"/>
       <c r="D32" s="3" t="s">
-        <v>152</v>
+        <v>46</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>263</v>
+        <v>220</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="22" t="s">
-        <v>332</v>
-      </c>
-      <c r="B33" s="29"/>
-      <c r="D33" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E33" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G33" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>265</v>
+      <c r="D33" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="12"/>
       <c r="D34" s="3" t="s">
-        <v>46</v>
+        <v>233</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>43</v>
+        <v>234</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>220</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B35" s="12"/>
-      <c r="D35" s="5" t="s">
-        <v>232</v>
-      </c>
-      <c r="E35" s="6" t="s">
-        <v>175</v>
+      <c r="A35" s="25" t="s">
+        <v>312</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>226</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>237</v>
+        <v>179</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>129</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="25" t="s">
-        <v>312</v>
+      <c r="A36" s="3" t="s">
+        <v>76</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>166</v>
+        <v>75</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>234</v>
-      </c>
-      <c r="G36" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>133</v>
+        <v>229</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>249</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>75</v>
+      <c r="A37" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>5</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>231</v>
+        <v>45</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="H37" s="4" t="s">
-        <v>180</v>
+        <v>44</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>272</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>334</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="G38" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>227</v>
+      <c r="A38" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E39" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>272</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>334</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>251</v>
+        <v>72</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>131</v>
+        <v>71</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H42" s="1"/>
+        <v>217</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="43" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>115</v>
+        <v>218</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>128</v>
+        <v>242</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>204</v>
+        <v>167</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>218</v>
+        <v>151</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>84</v>
+        <v>165</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>67</v>
+        <v>212</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>242</v>
+        <v>149</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="G46" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>208</v>
+        <v>148</v>
+      </c>
+      <c r="G46" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="H46" s="18" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>212</v>
-      </c>
       <c r="D47" s="3" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="G47" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>205</v>
+        <v>163</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="11"/>
       <c r="D48" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="E48" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="H48" s="4" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="D49" s="3" t="s">
-        <v>162</v>
-      </c>
       <c r="E49" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="G49" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="H49" s="18" t="s">
-        <v>267</v>
-      </c>
+        <v>219</v>
+      </c>
+      <c r="G49" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="20"/>
     </row>
     <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>172</v>
+      <c r="A50" s="14" t="s">
+        <v>258</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>173</v>
+        <v>259</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="G50" s="22" t="s">
-        <v>278</v>
-      </c>
-      <c r="H50" s="6" t="s">
-        <v>279</v>
+        <v>161</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="14" t="s">
-        <v>258</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>219</v>
+      <c r="A51" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="5" t="s">
-        <v>252</v>
+      <c r="A52" s="19" t="s">
+        <v>339</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="G52" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" s="20"/>
+        <v>273</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>228</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="53" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="19" t="s">
-        <v>339</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>273</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>202</v>
+      <c r="A53" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>262</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>185</v>
+        <v>22</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>186</v>
+        <v>23</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D54" s="15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E54" s="16" t="s">
-        <v>228</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="D54" s="32"/>
+      <c r="E54" s="33"/>
       <c r="G54" s="3" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>164</v>
+      <c r="A55" s="14" t="s">
+        <v>268</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>213</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>262</v>
-      </c>
-      <c r="G55" s="3" t="s">
-        <v>191</v>
-      </c>
-      <c r="H55" s="4" t="s">
-        <v>192</v>
-      </c>
+        <v>269</v>
+      </c>
+      <c r="D55" s="34"/>
+      <c r="E55" s="35"/>
     </row>
     <row r="56" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="14" t="s">
-        <v>268</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="D56" s="3"/>
-      <c r="E56" s="4"/>
-      <c r="G56" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H56" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="22" t="s">
+      <c r="A56" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B56" s="6" t="s">
         <v>260</v>
       </c>
-      <c r="D57" s="3"/>
-      <c r="E57" s="4"/>
-      <c r="G57" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="H57" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
+    </row>
+    <row r="57" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D58" s="30" t="s">
         <v>348</v>
@@ -3521,6 +3525,10 @@
       <c r="E96" s="6" t="s">
         <v>131</v>
       </c>
+      <c r="G96" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H96" s="1"/>
     </row>
     <row r="97" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
@@ -3535,6 +3543,12 @@
       <c r="E97" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="G97" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="H97" s="4" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
@@ -3549,10 +3563,12 @@
       <c r="E98" s="4" t="s">
         <v>141</v>
       </c>
-      <c r="G98" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="H98" s="1"/>
+      <c r="G98" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H98" s="6" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="99" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
@@ -3568,10 +3584,10 @@
         <v>217</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>117</v>
+        <v>235</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>115</v>
+        <v>206</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3588,10 +3604,10 @@
         <v>218</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>116</v>
+        <v>207</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3608,10 +3624,10 @@
         <v>167</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3627,11 +3643,11 @@
       <c r="E102" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="G102" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="H102" s="6" t="s">
-        <v>208</v>
+      <c r="G102" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="H102" s="4" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3647,11 +3663,11 @@
       <c r="E103" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="G103" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="H103" s="4" t="s">
-        <v>205</v>
+      <c r="G103" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="H103" s="18" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3661,11 +3677,11 @@
       <c r="E104" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="G104" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="H104" s="4" t="s">
-        <v>196</v>
+      <c r="G104" s="22" t="s">
+        <v>278</v>
+      </c>
+      <c r="H104" s="6" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3679,12 +3695,6 @@
       <c r="E105" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="G105" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="H105" s="18" t="s">
-        <v>267</v>
-      </c>
     </row>
     <row r="106" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
@@ -3699,12 +3709,10 @@
       <c r="E106" s="4" t="s">
         <v>219</v>
       </c>
-      <c r="G106" s="22" t="s">
-        <v>278</v>
-      </c>
-      <c r="H106" s="6" t="s">
-        <v>345</v>
-      </c>
+      <c r="G106" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H106" s="20"/>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
@@ -3719,6 +3727,12 @@
       <c r="E107" s="4" t="s">
         <v>161</v>
       </c>
+      <c r="G107" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H107" s="4" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="108" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="25" t="s">
@@ -3733,10 +3747,12 @@
       <c r="E108" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="G108" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="H108" s="20"/>
+      <c r="G108" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="H108" s="4" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="109" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="25" t="s">
@@ -3752,13 +3768,13 @@
         <v>228</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>147</v>
       </c>
@@ -3772,13 +3788,13 @@
         <v>262</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>187</v>
+        <v>22</v>
       </c>
       <c r="H110" s="4" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>164</v>
       </c>
@@ -3786,38 +3802,26 @@
         <v>213</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="H111" s="4" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
         <v>268</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="G112" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H112" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="113" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="22" t="s">
         <v>282</v>
       </c>
       <c r="B113" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="G113" s="3" t="s">
-        <v>194</v>
-      </c>
-      <c r="H113" s="4" t="s">
-        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add EN-Int-Undead Keyboard to IntelliJ
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -8,14 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9F9328-4E21-4E40-91FD-75E33086A4A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF195315-D3DE-4B17-942E-A91467A82FCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="255" windowWidth="38640" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1241,7 +1249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1278,16 +1286,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -1309,6 +1314,64 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Grafik 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C5189D3-3511-40CE-B4AD-4E2894FF4497}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId2"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13687425" y="1028700"/>
+          <a:ext cx="13525500" cy="4508500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1632,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J113"/>
+  <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A76" zoomScale="115" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E6" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="N36" sqref="N36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1649,21 +1712,23 @@
     <col min="7" max="7" width="37.5703125" style="2" customWidth="1"/>
     <col min="8" max="8" width="27.5703125" style="2" customWidth="1"/>
     <col min="9" max="9" width="22.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="43" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.42578125" style="2"/>
+    <col min="10" max="10" width="30.7109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.42578125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.42578125" style="2"/>
+    <col min="13" max="13" width="24" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="41.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="30" t="s">
+    <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D1" s="34" t="s">
         <v>347</v>
       </c>
-      <c r="E1" s="30"/>
-      <c r="I1" s="30" t="s">
-        <v>349</v>
-      </c>
-      <c r="J1" s="30"/>
-    </row>
-    <row r="2" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="34"/>
+    </row>
+    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1677,7 +1742,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1696,12 +1761,8 @@
       <c r="H3" s="4" t="s">
         <v>200</v>
       </c>
-      <c r="I3" s="31" t="s">
-        <v>311</v>
-      </c>
-      <c r="J3" s="31"/>
-    </row>
-    <row r="4" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>184</v>
       </c>
@@ -1720,14 +1781,8 @@
       <c r="H4" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>283</v>
-      </c>
-      <c r="J4" s="23" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>257</v>
       </c>
@@ -1746,14 +1801,8 @@
       <c r="H5" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="I5" s="24" t="s">
-        <v>284</v>
-      </c>
-      <c r="J5" s="24" t="s">
-        <v>290</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1772,14 +1821,8 @@
       <c r="H6" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>285</v>
-      </c>
-      <c r="J6" s="23" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1798,14 +1841,8 @@
       <c r="H7" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="I7" s="24" t="s">
-        <v>286</v>
-      </c>
-      <c r="J7" s="24" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1824,14 +1861,8 @@
       <c r="H8" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="J8" s="24" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>143</v>
       </c>
@@ -1851,7 +1882,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>199</v>
       </c>
@@ -1870,14 +1901,8 @@
       <c r="H10" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="I10" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
@@ -1896,14 +1921,8 @@
       <c r="H11" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="I11" s="24" t="s">
-        <v>307</v>
-      </c>
-      <c r="J11" s="24" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
         <v>274</v>
       </c>
@@ -1922,14 +1941,8 @@
       <c r="H12" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="I12" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="J12" s="24" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -1949,7 +1962,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>19</v>
       </c>
@@ -1968,14 +1981,8 @@
       <c r="H14" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="I14" s="23" t="s">
-        <v>294</v>
-      </c>
-      <c r="J14" s="23" t="s">
-        <v>297</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>254</v>
       </c>
@@ -1994,14 +2001,8 @@
       <c r="H15" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="I15" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="J15" s="24" t="s">
-        <v>298</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
         <v>276</v>
       </c>
@@ -2020,14 +2021,8 @@
       <c r="H16" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="I16" s="24" t="s">
-        <v>296</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>299</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
         <v>170</v>
       </c>
@@ -2040,14 +2035,8 @@
       <c r="H17" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="I17" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="J17" s="24" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>118</v>
       </c>
@@ -2064,14 +2053,8 @@
       <c r="H18" s="4" t="s">
         <v>216</v>
       </c>
-      <c r="I18" s="24" t="s">
-        <v>302</v>
-      </c>
-      <c r="J18" s="24" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>124</v>
       </c>
@@ -2091,7 +2074,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>123</v>
       </c>
@@ -2110,14 +2093,8 @@
       <c r="H20" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="I20" s="5" t="s">
-        <v>304</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>122</v>
       </c>
@@ -2137,7 +2114,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D22" s="3" t="s">
         <v>54</v>
       </c>
@@ -2150,12 +2127,8 @@
       <c r="H22" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="I22" s="31" t="s">
-        <v>315</v>
-      </c>
-      <c r="J22" s="31"/>
-    </row>
-    <row r="23" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>24</v>
       </c>
@@ -2171,14 +2144,8 @@
       <c r="H23" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="I23" s="24" t="s">
-        <v>318</v>
-      </c>
-      <c r="J23" s="28" t="s">
-        <v>319</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
         <v>329</v>
       </c>
@@ -2197,14 +2164,8 @@
       <c r="H24" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="I24" s="24" t="s">
-        <v>320</v>
-      </c>
-      <c r="J24" s="27" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
         <v>326</v>
       </c>
@@ -2224,7 +2185,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>157</v>
       </c>
@@ -2243,11 +2204,8 @@
       <c r="H26" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I26" s="27" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2266,11 +2224,8 @@
       <c r="H27" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I27" s="24" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>209</v>
       </c>
@@ -2289,11 +2244,8 @@
       <c r="H28" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="I28" s="24" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>154</v>
       </c>
@@ -2312,11 +2264,8 @@
       <c r="H29" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="I29" s="24" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>198</v>
       </c>
@@ -2335,11 +2284,8 @@
       <c r="H30" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="I30" s="24" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>28</v>
       </c>
@@ -2358,11 +2304,8 @@
       <c r="H31" s="6" t="s">
         <v>265</v>
       </c>
-      <c r="I31" s="24" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
         <v>332</v>
       </c>
@@ -2380,7 +2323,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="5" t="s">
         <v>232</v>
       </c>
@@ -2394,7 +2337,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
         <v>66</v>
       </c>
@@ -2412,7 +2355,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
         <v>312</v>
       </c>
@@ -2432,7 +2375,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>76</v>
       </c>
@@ -2452,7 +2395,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>4</v>
       </c>
@@ -2472,7 +2415,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>77</v>
       </c>
@@ -2486,7 +2429,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>78</v>
       </c>
@@ -2504,7 +2447,7 @@
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>79</v>
       </c>
@@ -2524,7 +2467,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>80</v>
       </c>
@@ -2544,7 +2487,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>81</v>
       </c>
@@ -2564,7 +2507,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>82</v>
       </c>
@@ -2584,7 +2527,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>83</v>
       </c>
@@ -2604,7 +2547,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>84</v>
       </c>
@@ -2624,7 +2567,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>165</v>
       </c>
@@ -2643,8 +2586,18 @@
       <c r="H46" s="18" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I46" s="34" t="s">
+        <v>349</v>
+      </c>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="34"/>
+      <c r="N46" s="34"/>
+      <c r="O46" s="34"/>
+      <c r="P46" s="34"/>
+    </row>
+    <row r="47" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D47" s="3" t="s">
         <v>162</v>
       </c>
@@ -2658,7 +2611,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>125</v>
       </c>
@@ -2669,8 +2622,19 @@
       <c r="E48" s="4" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I48" s="34" t="s">
+        <v>311</v>
+      </c>
+      <c r="J48" s="34"/>
+      <c r="K48" s="34"/>
+      <c r="L48" s="34"/>
+      <c r="M48" s="34"/>
+      <c r="O48" s="34" t="s">
+        <v>315</v>
+      </c>
+      <c r="P48" s="34"/>
+    </row>
+    <row r="49" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>172</v>
       </c>
@@ -2687,8 +2651,27 @@
         <v>21</v>
       </c>
       <c r="H49" s="20"/>
-    </row>
-    <row r="50" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I49" s="23" t="s">
+        <v>283</v>
+      </c>
+      <c r="J49" s="23" t="s">
+        <v>289</v>
+      </c>
+      <c r="K49" s="23"/>
+      <c r="L49" s="24" t="s">
+        <v>306</v>
+      </c>
+      <c r="M49" s="24" t="s">
+        <v>288</v>
+      </c>
+      <c r="O49" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="P49" s="28" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
         <v>258</v>
       </c>
@@ -2707,8 +2690,27 @@
       <c r="H50" s="4" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I50" s="24" t="s">
+        <v>284</v>
+      </c>
+      <c r="J50" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="K50" s="24"/>
+      <c r="L50" s="24" t="s">
+        <v>307</v>
+      </c>
+      <c r="M50" s="24" t="s">
+        <v>309</v>
+      </c>
+      <c r="O50" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="P50" s="27" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
         <v>252</v>
       </c>
@@ -2727,8 +2729,21 @@
       <c r="H51" s="4" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I51" s="23" t="s">
+        <v>285</v>
+      </c>
+      <c r="J51" s="23" t="s">
+        <v>291</v>
+      </c>
+      <c r="K51" s="23"/>
+      <c r="L51" s="24" t="s">
+        <v>308</v>
+      </c>
+      <c r="M51" s="24" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
         <v>339</v>
       </c>
@@ -2747,8 +2762,19 @@
       <c r="H52" s="4" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I52" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="J52" s="24" t="s">
+        <v>292</v>
+      </c>
+      <c r="K52" s="24"/>
+      <c r="O52" s="34" t="s">
+        <v>322</v>
+      </c>
+      <c r="P52" s="34"/>
+    </row>
+    <row r="53" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>147</v>
       </c>
@@ -2767,49 +2793,108 @@
       <c r="H53" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I53" s="24" t="s">
+        <v>287</v>
+      </c>
+      <c r="J53" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="K53" s="24"/>
+      <c r="L53" s="23" t="s">
+        <v>294</v>
+      </c>
+      <c r="M53" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="O53" s="24" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>164</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="D54" s="32"/>
-      <c r="E54" s="33"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="31"/>
       <c r="G54" s="3" t="s">
         <v>194</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L54" s="24" t="s">
+        <v>295</v>
+      </c>
+      <c r="M54" s="24" t="s">
+        <v>298</v>
+      </c>
+      <c r="O54" s="24" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
         <v>268</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="D55" s="34"/>
-      <c r="E55" s="35"/>
-    </row>
-    <row r="56" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="32"/>
+      <c r="E55" s="33"/>
+      <c r="I55" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J55" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="L55" s="24" t="s">
+        <v>296</v>
+      </c>
+      <c r="M55" s="24" t="s">
+        <v>299</v>
+      </c>
+      <c r="O55" s="24" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
         <v>282</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="30" t="s">
+      <c r="L56" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="M56" s="24" t="s">
+        <v>301</v>
+      </c>
+      <c r="O56" s="24" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L57" s="24" t="s">
+        <v>302</v>
+      </c>
+      <c r="M57" s="24" t="s">
+        <v>303</v>
+      </c>
+      <c r="O57" s="24" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D58" s="34" t="s">
         <v>348</v>
       </c>
-      <c r="E58" s="30"/>
-    </row>
-    <row r="59" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="34"/>
+    </row>
+    <row r="59" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>6</v>
       </c>
@@ -2823,7 +2908,7 @@
       </c>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>7</v>
       </c>
@@ -2843,7 +2928,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>184</v>
       </c>
@@ -2863,7 +2948,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>257</v>
       </c>
@@ -2883,7 +2968,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>9</v>
       </c>
@@ -2903,7 +2988,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>11</v>
       </c>
@@ -3825,17 +3910,19 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="I1:J1"/>
+  <mergeCells count="6">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="D58:E58"/>
-    <mergeCell ref="I22:J22"/>
-    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="O48:P48"/>
+    <mergeCell ref="I48:M48"/>
+    <mergeCell ref="I46:P46"/>
+    <mergeCell ref="O52:P52"/>
   </mergeCells>
   <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.196850393700787" footer="0.196850393700787"/>
   <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;LTool Windows: 1 Project / 2 Favorites / 3 Find / 4 Run / 5 Debug / 6 TODO / 7 Structure / 8 Services / 9 VCS / 0 Messages&amp;R&amp;"-,Fett"&amp;K00-037Shortcuts to remember &amp;K000000/&amp;K00-037 &amp;K03+027Changed or added &amp;K000000/&amp;K03+027 &amp;K06-019From Plugin</oddFooter>
   </headerFooter>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
docs: international symbols in keyboard layout
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF195315-D3DE-4B17-942E-A91467A82FCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD571621-6EE1-4EF8-B638-01CD1BB3A9CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="255" windowWidth="38640" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="255" windowWidth="38640" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1322,21 +1322,21 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>3067050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Grafik 2">
+        <xdr:cNvPr id="4" name="Grafik 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C5189D3-3511-40CE-B4AD-4E2894FF4497}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{77E2D10D-39FB-449C-B896-0ACDA0F36E69}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1361,8 +1361,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13687425" y="1028700"/>
-          <a:ext cx="13525500" cy="4508500"/>
+          <a:off x="13687425" y="0"/>
+          <a:ext cx="13506450" cy="4502150"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1697,8 +1697,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E6" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E1" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
update IntelliJ Shortcuts & Settings
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584476BF-27D9-4095-9FA5-687E75C408B8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1215E5-D288-45CD-A625-99A48AB231E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="255" windowWidth="38640" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="255" windowWidth="38640" windowHeight="20865" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="636" uniqueCount="349">
   <si>
     <t>Smart code completion</t>
   </si>
@@ -502,12 +502,6 @@
     <t>Ctrl + Alt + Shift + Mouse</t>
   </si>
   <si>
-    <t>Multiple Column Mode</t>
-  </si>
-  <si>
-    <t>Alt + Mouse</t>
-  </si>
-  <si>
     <t>Multiple Selection</t>
   </si>
   <si>
@@ -628,9 +622,6 @@
     <t>Go to class / Go to file</t>
   </si>
   <si>
-    <t>Ctrl + &lt; / Ctrl + Shift + &lt;</t>
-  </si>
-  <si>
     <t>Reset Font Size</t>
   </si>
   <si>
@@ -679,9 +670,6 @@
     <t>Ctrl + Shift + ↑/↓</t>
   </si>
   <si>
-    <t>Double Ctrl + ←/→/↑/↓</t>
-  </si>
-  <si>
     <t>Ctrl + Shift + ←/→/↑/↓</t>
   </si>
   <si>
@@ -752,9 +740,6 @@
   </si>
   <si>
     <t>Decrease/Increase Font Size</t>
-  </si>
-  <si>
-    <t>Ctrl + B; Ctrl + Click; Middle Click</t>
   </si>
   <si>
     <t>Ctrl + X; Shift + Delete</t>
@@ -1050,9 +1035,6 @@
     <t>Esc / F12</t>
   </si>
   <si>
-    <t>Go to next / prev highl. element usage</t>
-  </si>
-  <si>
     <t>Ctrl + , / Ctrl + Shift + ,</t>
   </si>
   <si>
@@ -1105,6 +1087,18 @@
   </si>
   <si>
     <t>Next / prev highlighted usage</t>
+  </si>
+  <si>
+    <t>Add or Remove Caret</t>
+  </si>
+  <si>
+    <t>Double Ctrl + ↑/↓</t>
+  </si>
+  <si>
+    <t>Add rectangular Selection on Mouse Drag</t>
+  </si>
+  <si>
+    <t>Ctrl + B; Ctrl + Click / Middle Click</t>
   </si>
 </sst>
 </file>
@@ -1692,8 +1686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A61" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A89" sqref="A89"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A61" zoomScale="130" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1719,7 +1713,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="34" t="s">
-        <v>347</v>
+        <v>341</v>
       </c>
       <c r="E1" s="34"/>
     </row>
@@ -1751,15 +1745,15 @@
         <v>30</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>158</v>
@@ -1779,10 +1773,10 @@
     </row>
     <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>64</v>
@@ -1791,10 +1785,10 @@
         <v>31</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1805,16 +1799,16 @@
         <v>10</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G6" s="25" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1845,10 +1839,10 @@
         <v>14</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>110</v>
@@ -1862,7 +1856,7 @@
         <v>143</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>63</v>
@@ -1871,18 +1865,18 @@
         <v>32</v>
       </c>
       <c r="G9" s="21" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>56</v>
@@ -1891,10 +1885,10 @@
         <v>36</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1919,7 +1913,7 @@
     </row>
     <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="19" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>137</v>
@@ -1928,7 +1922,7 @@
         <v>62</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>112</v>
@@ -1951,10 +1945,10 @@
         <v>33</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>244</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1979,16 +1973,16 @@
     </row>
     <row r="15" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>107</v>
@@ -1999,10 +1993,10 @@
     </row>
     <row r="16" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="14" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>59</v>
@@ -2019,13 +2013,13 @@
     </row>
     <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D17" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H17" s="4" t="s">
         <v>94</v>
@@ -2043,10 +2037,10 @@
         <v>126</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2066,7 +2060,7 @@
         <v>139</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2077,16 +2071,16 @@
         <v>120</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2134,18 +2128,18 @@
         <v>39</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="26" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>52</v>
@@ -2162,19 +2156,19 @@
     </row>
     <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H25" s="4" t="s">
         <v>98</v>
@@ -2191,7 +2185,7 @@
         <v>50</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>102</v>
@@ -2211,21 +2205,21 @@
         <v>49</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>48</v>
@@ -2234,10 +2228,10 @@
         <v>41</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2248,10 +2242,10 @@
         <v>155</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>100</v>
@@ -2262,10 +2256,10 @@
     </row>
     <row r="30" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>152</v>
@@ -2277,7 +2271,7 @@
         <v>134</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2294,15 +2288,15 @@
         <v>42</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="22" t="s">
-        <v>332</v>
+        <v>344</v>
       </c>
       <c r="B32" s="29"/>
       <c r="D32" s="3" t="s">
@@ -2315,18 +2309,18 @@
         <v>135</v>
       </c>
       <c r="H32" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D33" s="5" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H33" s="4" t="s">
         <v>129</v>
@@ -2338,10 +2332,10 @@
       </c>
       <c r="B34" s="12"/>
       <c r="D34" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G34" s="3" t="s">
         <v>132</v>
@@ -2352,22 +2346,22 @@
     </row>
     <row r="35" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2378,16 +2372,16 @@
         <v>75</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G36" s="13" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2404,24 +2398,24 @@
         <v>44</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2479,7 +2473,7 @@
         <v>116</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2493,13 +2487,13 @@
         <v>128</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H42" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2513,13 +2507,13 @@
         <v>136</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2530,16 +2524,16 @@
         <v>68</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H44" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2556,33 +2550,33 @@
         <v>151</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>148</v>
+        <v>346</v>
       </c>
       <c r="G46" s="17" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="I46" s="34" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="J46" s="34"/>
       <c r="K46" s="34"/>
@@ -2593,17 +2587,17 @@
       <c r="P46" s="34"/>
     </row>
     <row r="47" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D47" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E47" s="4" t="s">
-        <v>163</v>
+      <c r="D47" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>148</v>
       </c>
       <c r="G47" s="22" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2611,161 +2605,161 @@
         <v>125</v>
       </c>
       <c r="B48" s="11"/>
-      <c r="D48" s="3" t="s">
-        <v>160</v>
+      <c r="D48" s="25" t="s">
+        <v>345</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="I48" s="34" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="J48" s="34"/>
       <c r="K48" s="34"/>
       <c r="L48" s="34"/>
       <c r="M48" s="34"/>
       <c r="O48" s="34" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="P48" s="34"/>
     </row>
     <row r="49" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D49" s="3" t="s">
-        <v>149</v>
+        <v>171</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>347</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>219</v>
+        <v>159</v>
       </c>
       <c r="G49" s="11" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="20"/>
       <c r="I49" s="23" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="J49" s="23" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="K49" s="23"/>
       <c r="L49" s="24" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="M49" s="24" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="O49" s="24" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="P49" s="28" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="14" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>161</v>
+        <v>254</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E50" s="16" t="s">
+        <v>340</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H50" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="I50" s="24" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="J50" s="24" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="K50" s="24"/>
       <c r="L50" s="24" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="M50" s="24" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="O50" s="24" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="P50" s="27" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>202</v>
+      <c r="D51" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="E51" s="16" t="s">
+        <v>224</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="I51" s="23" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="J51" s="23" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="K51" s="23"/>
       <c r="L51" s="24" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="M51" s="24" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="19" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>203</v>
+        <v>256</v>
       </c>
       <c r="E52" s="16" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="I52" s="24" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="J52" s="24" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="K52" s="24"/>
       <c r="O52" s="34" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="P52" s="34"/>
     </row>
@@ -2776,12 +2770,8 @@
       <c r="B53" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D53" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="E53" s="16" t="s">
-        <v>262</v>
-      </c>
+      <c r="D53" s="30"/>
+      <c r="E53" s="31"/>
       <c r="G53" s="3" t="s">
         <v>22</v>
       </c>
@@ -2789,103 +2779,103 @@
         <v>23</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="J53" s="24" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="K53" s="24"/>
       <c r="L53" s="23" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="M53" s="23" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="O53" s="24" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D54" s="30"/>
       <c r="E54" s="31"/>
       <c r="G54" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="L54" s="24" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="M54" s="24" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="O54" s="24" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="14" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D55" s="32"/>
       <c r="E55" s="33"/>
       <c r="I55" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="L55" s="24" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="M55" s="24" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="O55" s="24" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="22" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="L56" s="24" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="M56" s="24" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="O56" s="24" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L57" s="24" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="M57" s="24" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="O57" s="24" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D58" s="34" t="s">
-        <v>348</v>
+        <v>342</v>
       </c>
       <c r="E58" s="34"/>
     </row>
@@ -2917,15 +2907,15 @@
         <v>30</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>158</v>
@@ -2945,10 +2935,10 @@
     </row>
     <row r="62" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>64</v>
@@ -2957,10 +2947,10 @@
         <v>31</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2971,16 +2961,16 @@
         <v>10</v>
       </c>
       <c r="D63" s="19" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G63" s="25" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>331</v>
+        <v>326</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3011,10 +3001,10 @@
         <v>14</v>
       </c>
       <c r="D65" s="26" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>110</v>
@@ -3028,7 +3018,7 @@
         <v>143</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>63</v>
@@ -3037,18 +3027,18 @@
         <v>32</v>
       </c>
       <c r="G66" s="21" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="D67" s="3" t="s">
         <v>56</v>
@@ -3057,10 +3047,10 @@
         <v>36</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3085,16 +3075,16 @@
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="D69" s="3" t="s">
         <v>62</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G69" s="3" t="s">
         <v>112</v>
@@ -3117,10 +3107,10 @@
         <v>33</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>244</v>
+        <v>348</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3145,16 +3135,16 @@
     </row>
     <row r="72" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G72" s="3" t="s">
         <v>107</v>
@@ -3165,10 +3155,10 @@
     </row>
     <row r="73" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="14" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D73" s="3" t="s">
         <v>59</v>
@@ -3185,13 +3175,13 @@
     </row>
     <row r="74" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D74" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H74" s="4" t="s">
         <v>94</v>
@@ -3209,10 +3199,10 @@
         <v>126</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3232,7 +3222,7 @@
         <v>139</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3243,16 +3233,16 @@
         <v>120</v>
       </c>
       <c r="D77" s="7" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="E77" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3300,18 +3290,18 @@
         <v>39</v>
       </c>
       <c r="G80" s="14" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="26" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>52</v>
@@ -3328,19 +3318,19 @@
     </row>
     <row r="82" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="26" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>51</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H82" s="4" t="s">
         <v>98</v>
@@ -3357,7 +3347,7 @@
         <v>50</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="G83" s="3" t="s">
         <v>102</v>
@@ -3377,21 +3367,21 @@
         <v>49</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>48</v>
@@ -3400,10 +3390,10 @@
         <v>41</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3414,10 +3404,10 @@
         <v>155</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="G86" s="3" t="s">
         <v>100</v>
@@ -3428,10 +3418,10 @@
     </row>
     <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D87" s="3" t="s">
         <v>152</v>
@@ -3443,7 +3433,7 @@
         <v>134</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3460,18 +3450,18 @@
         <v>42</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="22" t="s">
-        <v>350</v>
+        <v>344</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="D89" s="3" t="s">
         <v>46</v>
@@ -3483,18 +3473,18 @@
         <v>135</v>
       </c>
       <c r="H89" s="4" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D90" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="H90" s="4" t="s">
         <v>129</v>
@@ -3506,10 +3496,10 @@
       </c>
       <c r="B91" s="12"/>
       <c r="D91" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="G91" s="3" t="s">
         <v>132</v>
@@ -3520,22 +3510,22 @@
     </row>
     <row r="92" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="25" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3546,16 +3536,16 @@
         <v>75</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="G93" s="13" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3572,24 +3562,24 @@
         <v>44</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="H94" s="4" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="3" t="s">
+      <c r="A95" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B95" s="4" t="s">
+      <c r="B95" s="8" t="s">
         <v>74</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3647,7 +3637,7 @@
         <v>116</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3661,13 +3651,13 @@
         <v>128</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H99" s="4" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3681,13 +3671,13 @@
         <v>136</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="H100" s="6" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3698,16 +3688,16 @@
         <v>68</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="H101" s="4" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3724,44 +3714,44 @@
         <v>151</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D103" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="G103" s="17" t="s">
+        <v>261</v>
+      </c>
+      <c r="H103" s="18" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D104" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="E103" s="4" t="s">
+      <c r="E104" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G103" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="H103" s="18" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D104" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="E104" s="4" t="s">
-        <v>163</v>
-      </c>
       <c r="G104" s="22" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="H104" s="6" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3769,25 +3759,25 @@
         <v>125</v>
       </c>
       <c r="B105" s="11"/>
-      <c r="D105" s="3" t="s">
-        <v>160</v>
+      <c r="D105" s="25" t="s">
+        <v>345</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>149</v>
+        <v>171</v>
+      </c>
+      <c r="D106" s="25" t="s">
+        <v>347</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>219</v>
+        <v>159</v>
       </c>
       <c r="G106" s="11" t="s">
         <v>21</v>
@@ -3796,62 +3786,62 @@
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="14" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="D107" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="E107" s="4" t="s">
-        <v>161</v>
+        <v>254</v>
+      </c>
+      <c r="D107" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="E107" s="16" t="s">
+        <v>340</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="H107" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="25" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>340</v>
-      </c>
-      <c r="D108" s="5" t="s">
-        <v>243</v>
+        <v>334</v>
+      </c>
+      <c r="D108" s="15" t="s">
+        <v>200</v>
       </c>
       <c r="E108" s="16" t="s">
-        <v>346</v>
+        <v>224</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="25" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D109" s="15" t="s">
-        <v>203</v>
+        <v>256</v>
       </c>
       <c r="E109" s="16" t="s">
-        <v>228</v>
+        <v>257</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="H109" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3861,12 +3851,6 @@
       <c r="B110" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D110" s="15" t="s">
-        <v>261</v>
-      </c>
-      <c r="E110" s="16" t="s">
-        <v>262</v>
-      </c>
       <c r="G110" s="3" t="s">
         <v>22</v>
       </c>
@@ -3876,32 +3860,32 @@
     </row>
     <row r="111" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="H111" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="14" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
     </row>
     <row r="113" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="22" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add IntelliJ Plugin String Manipulation
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\IntelliJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\ubuntu\projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5673477F-6D96-4E2C-B739-4FD76EEDE3A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC22B0B9-3A2A-4A46-91F2-D4EF5716B494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30600" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="357">
   <si>
     <t>Smart code completion</t>
   </si>
@@ -1117,6 +1117,12 @@
   </si>
   <si>
     <t>Scroll to Center</t>
+  </si>
+  <si>
+    <t>String Manipulation</t>
+  </si>
+  <si>
+    <t>Alt + M</t>
   </si>
 </sst>
 </file>
@@ -1256,7 +1262,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1297,6 +1303,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -1701,8 +1709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A24" zoomScale="115" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
-      <selection activeCell="G36" sqref="G36:H36"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A70" zoomScale="115" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="115" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2785,8 +2793,12 @@
       <c r="B53" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
+      <c r="D53" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="E53" s="33" t="s">
+        <v>356</v>
+      </c>
       <c r="G53" s="3" t="s">
         <v>187</v>
       </c>
@@ -3877,6 +3889,12 @@
       </c>
       <c r="B110" s="4" t="s">
         <v>146</v>
+      </c>
+      <c r="D110" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="E110" s="33" t="s">
+        <v>356</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>187</v>

</xml_diff>

<commit_message>
update IntelliJ Shortcuts to v2022.2
* JetBrains added shortcut for Increase/Decrease Font Size
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\ubuntu\projects\wiki\Settings\IntelliJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29936540-57E3-427D-B6E3-8B6718D43AE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A09139-4779-4AC2-883C-6F0FC5F2F605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1068,9 +1068,6 @@
     <t>Ctrl + Shift + ;</t>
   </si>
   <si>
-    <t>Ctrl + \ / Ctrl + Shift + \</t>
-  </si>
-  <si>
     <t>IntelliJ Shortcuts Deutsch</t>
   </si>
   <si>
@@ -1129,6 +1126,9 @@
   </si>
   <si>
     <t>Open Recent (Project)</t>
+  </si>
+  <si>
+    <t>Alt + Shift + ,/.</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -1240,15 +1240,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -1268,7 +1259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1288,11 +1279,10 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1715,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A46" zoomScale="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A64" sqref="A64"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A40" zoomScale="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1741,10 +1731,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="33" t="s">
-        <v>339</v>
-      </c>
-      <c r="E1" s="33"/>
+      <c r="D1" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="E1" s="32"/>
     </row>
     <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1827,13 +1817,13 @@
       <c r="B6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="17" t="s">
         <v>264</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="23" t="s">
         <v>323</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -1867,11 +1857,11 @@
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="25" t="s">
-        <v>352</v>
+      <c r="D8" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>110</v>
@@ -1887,13 +1877,13 @@
       <c r="B9" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>306</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>273</v>
       </c>
       <c r="H9" s="8" t="s">
@@ -1941,7 +1931,7 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="17" t="s">
         <v>267</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -1977,7 +1967,7 @@
         <v>241</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2041,11 +2031,11 @@
       </c>
     </row>
     <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>358</v>
+      <c r="A17" s="17" t="s">
+        <v>357</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>59</v>
@@ -2093,7 +2083,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="24" t="s">
+      <c r="A20" s="23" t="s">
         <v>124</v>
       </c>
       <c r="B20" s="4" t="s">
@@ -2184,7 +2174,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="25" t="s">
+      <c r="A25" s="24" t="s">
         <v>322</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -2204,7 +2194,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="24" t="s">
         <v>319</v>
       </c>
       <c r="B26" s="8" t="s">
@@ -2344,10 +2334,10 @@
       </c>
     </row>
     <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="21" t="s">
-        <v>342</v>
-      </c>
-      <c r="B33" s="28"/>
+      <c r="A33" s="20" t="s">
+        <v>341</v>
+      </c>
+      <c r="B33" s="27"/>
       <c r="D33" s="3" t="s">
         <v>46</v>
       </c>
@@ -2394,7 +2384,7 @@
       </c>
     </row>
     <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="24" t="s">
+      <c r="A36" s="23" t="s">
         <v>305</v>
       </c>
       <c r="B36" s="4" t="s">
@@ -2406,11 +2396,11 @@
       <c r="E36" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="G36" s="23" t="s">
-        <v>354</v>
-      </c>
-      <c r="H36" s="27" t="s">
+      <c r="G36" s="22" t="s">
         <v>353</v>
+      </c>
+      <c r="H36" s="26" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2604,16 +2594,16 @@
       <c r="H46" s="4" t="s">
         <v>192</v>
       </c>
-      <c r="I46" s="33" t="s">
-        <v>341</v>
-      </c>
-      <c r="J46" s="33"/>
-      <c r="K46" s="33"/>
-      <c r="L46" s="33"/>
-      <c r="M46" s="33"/>
-      <c r="N46" s="33"/>
-      <c r="O46" s="33"/>
-      <c r="P46" s="33"/>
+      <c r="I46" s="32" t="s">
+        <v>340</v>
+      </c>
+      <c r="J46" s="32"/>
+      <c r="K46" s="32"/>
+      <c r="L46" s="32"/>
+      <c r="M46" s="32"/>
+      <c r="N46" s="32"/>
+      <c r="O46" s="32"/>
+      <c r="P46" s="32"/>
     </row>
     <row r="47" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
@@ -2626,12 +2616,12 @@
         <v>159</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="G47" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G47" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="H47" s="17" t="s">
+      <c r="H47" s="16" t="s">
         <v>260</v>
       </c>
     </row>
@@ -2642,52 +2632,52 @@
       <c r="E48" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G48" s="21" t="s">
+      <c r="G48" s="20" t="s">
         <v>271</v>
       </c>
       <c r="H48" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="I48" s="33" t="s">
+      <c r="I48" s="32" t="s">
         <v>304</v>
       </c>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="33"/>
-      <c r="M48" s="33"/>
-      <c r="O48" s="33" t="s">
+      <c r="J48" s="32"/>
+      <c r="K48" s="32"/>
+      <c r="L48" s="32"/>
+      <c r="M48" s="32"/>
+      <c r="O48" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="P48" s="33"/>
+      <c r="P48" s="32"/>
     </row>
     <row r="49" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>125</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="D49" s="24" t="s">
-        <v>343</v>
+      <c r="D49" s="23" t="s">
+        <v>342</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="I49" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="I49" s="21" t="s">
         <v>276</v>
       </c>
-      <c r="J49" s="22" t="s">
+      <c r="J49" s="21" t="s">
         <v>282</v>
       </c>
-      <c r="K49" s="22"/>
-      <c r="L49" s="23" t="s">
+      <c r="K49" s="21"/>
+      <c r="L49" s="22" t="s">
         <v>299</v>
       </c>
-      <c r="M49" s="23" t="s">
+      <c r="M49" s="22" t="s">
         <v>281</v>
       </c>
-      <c r="O49" s="23" t="s">
+      <c r="O49" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="P49" s="27" t="s">
+      <c r="P49" s="26" t="s">
         <v>312</v>
       </c>
     </row>
@@ -2698,33 +2688,33 @@
       <c r="B50" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D50" s="24" t="s">
-        <v>348</v>
+      <c r="D50" s="23" t="s">
+        <v>347</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G50" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H50" s="19"/>
-      <c r="I50" s="23" t="s">
+      <c r="H50" s="18"/>
+      <c r="I50" s="22" t="s">
         <v>277</v>
       </c>
-      <c r="J50" s="23" t="s">
+      <c r="J50" s="22" t="s">
         <v>283</v>
       </c>
-      <c r="K50" s="23"/>
-      <c r="L50" s="23" t="s">
+      <c r="K50" s="22"/>
+      <c r="L50" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="M50" s="23" t="s">
+      <c r="M50" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="O50" s="23" t="s">
+      <c r="O50" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="P50" s="26" t="s">
+      <c r="P50" s="25" t="s">
         <v>314</v>
       </c>
     </row>
@@ -2735,11 +2725,11 @@
       <c r="B51" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="E51" s="15" t="s">
-        <v>338</v>
+      <c r="E51" s="4" t="s">
+        <v>358</v>
       </c>
       <c r="G51" s="3" t="s">
         <v>181</v>
@@ -2747,17 +2737,17 @@
       <c r="H51" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="I51" s="22" t="s">
+      <c r="I51" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="J51" s="22" t="s">
+      <c r="J51" s="21" t="s">
         <v>284</v>
       </c>
-      <c r="K51" s="22"/>
-      <c r="L51" s="23" t="s">
+      <c r="K51" s="21"/>
+      <c r="L51" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="M51" s="23" t="s">
+      <c r="M51" s="22" t="s">
         <v>303</v>
       </c>
     </row>
@@ -2780,30 +2770,30 @@
       <c r="H52" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="I52" s="23" t="s">
+      <c r="I52" s="22" t="s">
         <v>279</v>
       </c>
-      <c r="J52" s="23" t="s">
+      <c r="J52" s="22" t="s">
         <v>285</v>
       </c>
-      <c r="K52" s="23"/>
-      <c r="O52" s="33" t="s">
+      <c r="K52" s="22"/>
+      <c r="O52" s="32" t="s">
         <v>315</v>
       </c>
-      <c r="P52" s="33"/>
+      <c r="P52" s="32"/>
     </row>
     <row r="53" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="17" t="s">
         <v>331</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>266</v>
       </c>
-      <c r="D53" s="31" t="s">
+      <c r="D53" s="30" t="s">
+        <v>354</v>
+      </c>
+      <c r="E53" s="31" t="s">
         <v>355</v>
-      </c>
-      <c r="E53" s="32" t="s">
-        <v>356</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>187</v>
@@ -2811,20 +2801,20 @@
       <c r="H53" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="I53" s="23" t="s">
+      <c r="I53" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="J53" s="23" t="s">
+      <c r="J53" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="K53" s="23"/>
-      <c r="L53" s="22" t="s">
+      <c r="K53" s="22"/>
+      <c r="L53" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="M53" s="22" t="s">
+      <c r="M53" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="O53" s="23" t="s">
+      <c r="O53" s="22" t="s">
         <v>309</v>
       </c>
     </row>
@@ -2835,21 +2825,21 @@
       <c r="B54" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D54" s="29"/>
-      <c r="E54" s="30"/>
+      <c r="D54" s="28"/>
+      <c r="E54" s="29"/>
       <c r="G54" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L54" s="23" t="s">
+      <c r="L54" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="M54" s="23" t="s">
+      <c r="M54" s="22" t="s">
         <v>291</v>
       </c>
-      <c r="O54" s="23" t="s">
+      <c r="O54" s="22" t="s">
         <v>310</v>
       </c>
     </row>
@@ -2860,8 +2850,8 @@
       <c r="B55" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="D55" s="29"/>
-      <c r="E55" s="30"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="29"/>
       <c r="G55" s="3" t="s">
         <v>190</v>
       </c>
@@ -2874,13 +2864,13 @@
       <c r="J55" s="5" t="s">
         <v>298</v>
       </c>
-      <c r="L55" s="23" t="s">
+      <c r="L55" s="22" t="s">
         <v>289</v>
       </c>
-      <c r="M55" s="23" t="s">
+      <c r="M55" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="O55" s="23" t="s">
+      <c r="O55" s="22" t="s">
         <v>317</v>
       </c>
     </row>
@@ -2891,18 +2881,18 @@
       <c r="B56" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="L56" s="23" t="s">
+      <c r="L56" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="M56" s="23" t="s">
+      <c r="M56" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="O56" s="23" t="s">
+      <c r="O56" s="22" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="21" t="s">
+      <c r="A57" s="20" t="s">
         <v>275</v>
       </c>
       <c r="B57" s="6" t="s">
@@ -2914,21 +2904,21 @@
       <c r="E57" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="L57" s="23" t="s">
+      <c r="L57" s="22" t="s">
         <v>295</v>
       </c>
-      <c r="M57" s="23" t="s">
+      <c r="M57" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="O57" s="23" t="s">
+      <c r="O57" s="22" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="33" t="s">
-        <v>340</v>
-      </c>
-      <c r="E58" s="33"/>
+      <c r="D58" s="32" t="s">
+        <v>339</v>
+      </c>
+      <c r="E58" s="32"/>
     </row>
     <row r="59" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -3011,13 +3001,13 @@
       <c r="B63" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D63" s="18" t="s">
+      <c r="D63" s="17" t="s">
         <v>264</v>
       </c>
       <c r="E63" s="6" t="s">
         <v>263</v>
       </c>
-      <c r="G63" s="24" t="s">
+      <c r="G63" s="23" t="s">
         <v>323</v>
       </c>
       <c r="H63" s="4" t="s">
@@ -3031,8 +3021,8 @@
       <c r="B64" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D64" s="25" t="s">
-        <v>350</v>
+      <c r="D64" s="24" t="s">
+        <v>349</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>3</v>
@@ -3051,11 +3041,11 @@
       <c r="B65" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="25" t="s">
-        <v>352</v>
+      <c r="D65" s="24" t="s">
+        <v>351</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="G65" s="3" t="s">
         <v>110</v>
@@ -3071,13 +3061,13 @@
       <c r="B66" s="4" t="s">
         <v>328</v>
       </c>
-      <c r="D66" s="25" t="s">
+      <c r="D66" s="24" t="s">
         <v>306</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>307</v>
       </c>
-      <c r="G66" s="20" t="s">
+      <c r="G66" s="19" t="s">
         <v>273</v>
       </c>
       <c r="H66" s="8" t="s">
@@ -3161,7 +3151,7 @@
         <v>241</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3225,11 +3215,11 @@
       </c>
     </row>
     <row r="74" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="18" t="s">
-        <v>358</v>
+      <c r="A74" s="17" t="s">
+        <v>357</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="D74" s="3" t="s">
         <v>59</v>
@@ -3269,7 +3259,7 @@
       <c r="E76" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="G76" s="24" t="s">
+      <c r="G76" s="23" t="s">
         <v>139</v>
       </c>
       <c r="H76" s="4" t="s">
@@ -3277,7 +3267,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="24" t="s">
+      <c r="A77" s="23" t="s">
         <v>124</v>
       </c>
       <c r="B77" s="4" t="s">
@@ -3323,8 +3313,8 @@
       <c r="B79" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="D79" s="24" t="s">
-        <v>349</v>
+      <c r="D79" s="23" t="s">
+        <v>348</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>37</v>
@@ -3368,7 +3358,7 @@
       </c>
     </row>
     <row r="82" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="25" t="s">
+      <c r="A82" s="24" t="s">
         <v>322</v>
       </c>
       <c r="B82" s="8" t="s">
@@ -3388,7 +3378,7 @@
       </c>
     </row>
     <row r="83" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="25" t="s">
+      <c r="A83" s="24" t="s">
         <v>319</v>
       </c>
       <c r="B83" s="8" t="s">
@@ -3528,8 +3518,8 @@
       </c>
     </row>
     <row r="90" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="21" t="s">
-        <v>342</v>
+      <c r="A90" s="20" t="s">
+        <v>341</v>
       </c>
       <c r="B90" s="6" t="s">
         <v>325</v>
@@ -3580,7 +3570,7 @@
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="24" t="s">
+      <c r="A93" s="23" t="s">
         <v>305</v>
       </c>
       <c r="B93" s="4" t="s">
@@ -3592,11 +3582,11 @@
       <c r="E93" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="G93" s="23" t="s">
-        <v>354</v>
-      </c>
-      <c r="H93" s="27" t="s">
+      <c r="G93" s="22" t="s">
         <v>353</v>
+      </c>
+      <c r="H93" s="26" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3802,12 +3792,12 @@
         <v>159</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>344</v>
-      </c>
-      <c r="G104" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="G104" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="H104" s="17" t="s">
+      <c r="H104" s="16" t="s">
         <v>260</v>
       </c>
     </row>
@@ -3818,7 +3808,7 @@
       <c r="E105" s="8" t="s">
         <v>148</v>
       </c>
-      <c r="G105" s="21" t="s">
+      <c r="G105" s="20" t="s">
         <v>271</v>
       </c>
       <c r="H105" s="6" t="s">
@@ -3830,11 +3820,11 @@
         <v>125</v>
       </c>
       <c r="B106" s="11"/>
-      <c r="D106" s="24" t="s">
-        <v>343</v>
+      <c r="D106" s="23" t="s">
+        <v>342</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3844,16 +3834,16 @@
       <c r="B107" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="D107" s="24" t="s">
-        <v>348</v>
+      <c r="D107" s="23" t="s">
+        <v>347</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="H107" s="19"/>
+      <c r="H107" s="18"/>
     </row>
     <row r="108" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
@@ -3862,11 +3852,11 @@
       <c r="B108" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D108" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="E108" s="15" t="s">
-        <v>338</v>
+      <c r="E108" s="4" t="s">
+        <v>358</v>
       </c>
       <c r="G108" s="3" t="s">
         <v>181</v>
@@ -3876,7 +3866,7 @@
       </c>
     </row>
     <row r="109" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="24" t="s">
+      <c r="A109" s="23" t="s">
         <v>245</v>
       </c>
       <c r="B109" s="4" t="s">
@@ -3896,17 +3886,17 @@
       </c>
     </row>
     <row r="110" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="24" t="s">
+      <c r="A110" s="23" t="s">
         <v>331</v>
       </c>
       <c r="B110" s="4" t="s">
         <v>327</v>
       </c>
-      <c r="D110" s="31" t="s">
+      <c r="D110" s="30" t="s">
+        <v>354</v>
+      </c>
+      <c r="E110" s="31" t="s">
         <v>355</v>
-      </c>
-      <c r="E110" s="32" t="s">
-        <v>356</v>
       </c>
       <c r="G110" s="3" t="s">
         <v>187</v>
@@ -3952,7 +3942,7 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="21" t="s">
+      <c r="A114" s="20" t="s">
         <v>275</v>
       </c>
       <c r="B114" s="6" t="s">

</xml_diff>

<commit_message>
feat: add IntelliJ Shortcut
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28A09139-4779-4AC2-883C-6F0FC5F2F605}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174131D5-7025-441A-BCD4-4A63D76B4CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -71,18 +71,6 @@
   </si>
   <si>
     <t>Alt + Shift + I</t>
-  </si>
-  <si>
-    <t>Open Settings dialog</t>
-  </si>
-  <si>
-    <t>Ctrl + Alt + S</t>
-  </si>
-  <si>
-    <t>Open Project Structure dialog</t>
-  </si>
-  <si>
-    <t>Ctrl + Alt + Shift + S</t>
   </si>
   <si>
     <t>Debugging</t>
@@ -1129,6 +1117,18 @@
   </si>
   <si>
     <t>Alt + Shift + ,/.</t>
+  </si>
+  <si>
+    <t>Ctrl + Alt (+ Shift) + S</t>
+  </si>
+  <si>
+    <t>Open Settings (Project Structure) dialog</t>
+  </si>
+  <si>
+    <t>Alt + \</t>
+  </si>
+  <si>
+    <t>Main Menu</t>
   </si>
 </sst>
 </file>
@@ -1259,7 +1259,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1286,21 +1286,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
@@ -1383,9 +1376,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1423,9 +1416,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1458,26 +1451,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1510,26 +1486,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1705,8 +1664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A40" zoomScale="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A51" zoomScale="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1731,10 +1690,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="32" t="s">
-        <v>338</v>
-      </c>
-      <c r="E1" s="32"/>
+      <c r="D1" s="24" t="s">
+        <v>334</v>
+      </c>
+      <c r="E1" s="24"/>
     </row>
     <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1742,11 +1701,11 @@
       </c>
       <c r="B2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -1758,24 +1717,24 @@
         <v>8</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>0</v>
@@ -1784,30 +1743,30 @@
         <v>1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1818,16 +1777,16 @@
         <v>10</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G6" s="23" t="s">
-        <v>323</v>
+        <v>259</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>319</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1844,10 +1803,10 @@
         <v>3</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1857,57 +1816,57 @@
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>351</v>
+      <c r="D8" s="19" t="s">
+        <v>347</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9" s="24" t="s">
-        <v>306</v>
+        <v>169</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>302</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B10" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H10" s="4" t="s">
         <v>206</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>234</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1918,509 +1877,509 @@
         <v>16</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
+      <c r="A13" s="25" t="s">
+        <v>356</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>18</v>
+        <v>355</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
-        <v>19</v>
+      <c r="A14" s="14" t="s">
+        <v>243</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>20</v>
+        <v>242</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>270</v>
+      <c r="A16" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>352</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>356</v>
+      <c r="B17" s="4" t="s">
+        <v>358</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H17" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H18" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B19" s="11"/>
       <c r="D19" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="23" t="s">
-        <v>124</v>
+      <c r="A20" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H20" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H21" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H22" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D23" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H23" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H24" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="24" t="s">
-        <v>322</v>
+      <c r="A25" s="19" t="s">
+        <v>318</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H25" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G26" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="24" t="s">
-        <v>319</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="H26" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H27" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H29" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H30" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E32" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="D33" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H32" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="B33" s="27"/>
-      <c r="D33" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E33" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H33" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D34" s="5" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H34" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B35" s="12"/>
       <c r="D35" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H35" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="23" t="s">
-        <v>305</v>
+      <c r="A36" s="14" t="s">
+        <v>301</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G36" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="H36" s="26" t="s">
-        <v>352</v>
+        <v>216</v>
+      </c>
+      <c r="G36" t="s">
+        <v>349</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="37" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G37" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="38" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2431,494 +2390,492 @@
         <v>5</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
     </row>
     <row r="39" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="40" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H40" s="1"/>
     </row>
     <row r="41" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H41" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G42" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="43" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="H43" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="44" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="45" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H45" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H46" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="I46" s="32" t="s">
-        <v>340</v>
-      </c>
-      <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-      <c r="M46" s="32"/>
-      <c r="N46" s="32"/>
-      <c r="O46" s="32"/>
-      <c r="P46" s="32"/>
+        <v>188</v>
+      </c>
+      <c r="I46" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="J46" s="24"/>
+      <c r="K46" s="24"/>
+      <c r="L46" s="24"/>
+      <c r="M46" s="24"/>
+      <c r="N46" s="24"/>
+      <c r="O46" s="24"/>
+      <c r="P46" s="24"/>
     </row>
     <row r="47" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G47" s="15" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H47" s="16" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="48" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D48" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E48" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G48" s="20" t="s">
-        <v>271</v>
+        <v>144</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>267</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="I48" s="32" t="s">
+        <v>268</v>
+      </c>
+      <c r="I48" s="24" t="s">
+        <v>300</v>
+      </c>
+      <c r="J48" s="24"/>
+      <c r="K48" s="24"/>
+      <c r="L48" s="24"/>
+      <c r="M48" s="24"/>
+      <c r="O48" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-      <c r="M48" s="32"/>
-      <c r="O48" s="32" t="s">
-        <v>308</v>
-      </c>
-      <c r="P48" s="32"/>
+      <c r="P48" s="24"/>
     </row>
     <row r="49" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B49" s="11"/>
-      <c r="D49" s="23" t="s">
-        <v>342</v>
+      <c r="D49" s="14" t="s">
+        <v>338</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>345</v>
-      </c>
-      <c r="I49" s="21" t="s">
-        <v>276</v>
-      </c>
-      <c r="J49" s="21" t="s">
-        <v>282</v>
-      </c>
-      <c r="K49" s="21"/>
-      <c r="L49" s="22" t="s">
-        <v>299</v>
-      </c>
-      <c r="M49" s="22" t="s">
-        <v>281</v>
-      </c>
-      <c r="O49" s="22" t="s">
-        <v>311</v>
-      </c>
-      <c r="P49" s="26" t="s">
-        <v>312</v>
+        <v>341</v>
+      </c>
+      <c r="I49" t="s">
+        <v>272</v>
+      </c>
+      <c r="J49" t="s">
+        <v>278</v>
+      </c>
+      <c r="K49"/>
+      <c r="L49" t="s">
+        <v>295</v>
+      </c>
+      <c r="M49" t="s">
+        <v>277</v>
+      </c>
+      <c r="O49" t="s">
+        <v>307</v>
+      </c>
+      <c r="P49" s="20" t="s">
+        <v>308</v>
       </c>
     </row>
     <row r="50" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D50" s="23" t="s">
-        <v>347</v>
+        <v>165</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>343</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G50" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H50" s="18"/>
-      <c r="I50" s="22" t="s">
-        <v>277</v>
-      </c>
-      <c r="J50" s="22" t="s">
-        <v>283</v>
-      </c>
-      <c r="K50" s="22"/>
-      <c r="L50" s="22" t="s">
-        <v>300</v>
-      </c>
-      <c r="M50" s="22" t="s">
-        <v>302</v>
-      </c>
-      <c r="O50" s="22" t="s">
-        <v>313</v>
-      </c>
-      <c r="P50" s="25" t="s">
-        <v>314</v>
+      <c r="I50" t="s">
+        <v>273</v>
+      </c>
+      <c r="J50" t="s">
+        <v>279</v>
+      </c>
+      <c r="K50"/>
+      <c r="L50" t="s">
+        <v>296</v>
+      </c>
+      <c r="M50" t="s">
+        <v>298</v>
+      </c>
+      <c r="O50" t="s">
+        <v>309</v>
+      </c>
+      <c r="P50" s="20" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="51" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="D51" s="23" t="s">
-        <v>237</v>
+        <v>248</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>233</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H51" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="I51" s="21" t="s">
-        <v>278</v>
-      </c>
-      <c r="J51" s="21" t="s">
-        <v>284</v>
-      </c>
-      <c r="K51" s="21"/>
-      <c r="L51" s="22" t="s">
-        <v>301</v>
-      </c>
-      <c r="M51" s="22" t="s">
-        <v>303</v>
+        <v>178</v>
+      </c>
+      <c r="I51" t="s">
+        <v>274</v>
+      </c>
+      <c r="J51" t="s">
+        <v>280</v>
+      </c>
+      <c r="K51"/>
+      <c r="L51" t="s">
+        <v>297</v>
+      </c>
+      <c r="M51" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="52" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="H52" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="I52" s="22" t="s">
-        <v>279</v>
-      </c>
-      <c r="J52" s="22" t="s">
-        <v>285</v>
-      </c>
-      <c r="K52" s="22"/>
-      <c r="O52" s="32" t="s">
-        <v>315</v>
-      </c>
-      <c r="P52" s="32"/>
+        <v>180</v>
+      </c>
+      <c r="I52" t="s">
+        <v>275</v>
+      </c>
+      <c r="J52" t="s">
+        <v>281</v>
+      </c>
+      <c r="K52"/>
+      <c r="O52" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="P52" s="24"/>
     </row>
     <row r="53" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="D53" s="30" t="s">
-        <v>354</v>
-      </c>
-      <c r="E53" s="31" t="s">
-        <v>355</v>
+        <v>262</v>
+      </c>
+      <c r="D53" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E53" s="23" t="s">
+        <v>351</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="H53" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="I53" s="22" t="s">
-        <v>280</v>
-      </c>
-      <c r="J53" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="I53" t="s">
+        <v>276</v>
+      </c>
+      <c r="J53" t="s">
+        <v>282</v>
+      </c>
+      <c r="K53"/>
+      <c r="L53" t="s">
+        <v>283</v>
+      </c>
+      <c r="M53" t="s">
         <v>286</v>
       </c>
-      <c r="K53" s="22"/>
-      <c r="L53" s="21" t="s">
-        <v>287</v>
-      </c>
-      <c r="M53" s="21" t="s">
-        <v>290</v>
-      </c>
-      <c r="O53" s="22" t="s">
-        <v>309</v>
+      <c r="O53" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="54" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="D54" s="28"/>
-      <c r="E54" s="29"/>
+        <v>142</v>
+      </c>
+      <c r="E54" s="20"/>
       <c r="G54" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H54" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="L54" s="22" t="s">
-        <v>288</v>
-      </c>
-      <c r="M54" s="22" t="s">
-        <v>291</v>
-      </c>
-      <c r="O54" s="22" t="s">
-        <v>310</v>
+        <v>19</v>
+      </c>
+      <c r="L54" t="s">
+        <v>284</v>
+      </c>
+      <c r="M54" t="s">
+        <v>287</v>
+      </c>
+      <c r="O54" t="s">
+        <v>306</v>
       </c>
     </row>
     <row r="55" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="D55" s="28"/>
-      <c r="E55" s="29"/>
+        <v>204</v>
+      </c>
+      <c r="E55" s="20"/>
       <c r="G55" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H55" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>298</v>
-      </c>
-      <c r="L55" s="22" t="s">
-        <v>289</v>
-      </c>
-      <c r="M55" s="22" t="s">
-        <v>292</v>
-      </c>
-      <c r="O55" s="22" t="s">
-        <v>317</v>
+        <v>294</v>
+      </c>
+      <c r="L55" t="s">
+        <v>285</v>
+      </c>
+      <c r="M55" t="s">
+        <v>288</v>
+      </c>
+      <c r="O55" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="56" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="L56" s="22" t="s">
-        <v>293</v>
-      </c>
-      <c r="M56" s="22" t="s">
-        <v>294</v>
-      </c>
-      <c r="O56" s="22" t="s">
-        <v>316</v>
+        <v>258</v>
+      </c>
+      <c r="L56" t="s">
+        <v>289</v>
+      </c>
+      <c r="M56" t="s">
+        <v>290</v>
+      </c>
+      <c r="O56" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="57" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
-        <v>275</v>
+      <c r="A57" s="17" t="s">
+        <v>271</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="L57" s="22" t="s">
-        <v>295</v>
-      </c>
-      <c r="M57" s="22" t="s">
-        <v>296</v>
-      </c>
-      <c r="O57" s="22" t="s">
-        <v>318</v>
+        <v>251</v>
+      </c>
+      <c r="L57" t="s">
+        <v>291</v>
+      </c>
+      <c r="M57" t="s">
+        <v>292</v>
+      </c>
+      <c r="O57" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="32" t="s">
-        <v>339</v>
-      </c>
-      <c r="E58" s="32"/>
+      <c r="D58" s="24" t="s">
+        <v>335</v>
+      </c>
+      <c r="E58" s="24"/>
     </row>
     <row r="59" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
@@ -2926,11 +2883,11 @@
       </c>
       <c r="B59" s="1"/>
       <c r="D59" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E59" s="1"/>
       <c r="G59" s="1" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="H59" s="1"/>
     </row>
@@ -2942,24 +2899,24 @@
         <v>8</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="H60" s="4" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="D61" s="7" t="s">
         <v>0</v>
@@ -2968,30 +2925,30 @@
         <v>1</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H61" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="62" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H62" s="4" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="63" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3002,16 +2959,16 @@
         <v>10</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="G63" s="23" t="s">
-        <v>323</v>
+        <v>259</v>
+      </c>
+      <c r="G63" s="14" t="s">
+        <v>319</v>
       </c>
       <c r="H63" s="4" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="64" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3021,17 +2978,17 @@
       <c r="B64" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D64" s="24" t="s">
-        <v>349</v>
+      <c r="D64" s="19" t="s">
+        <v>345</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>3</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H64" s="4" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3041,57 +2998,57 @@
       <c r="B65" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D65" s="24" t="s">
-        <v>351</v>
+      <c r="D65" s="19" t="s">
+        <v>347</v>
       </c>
       <c r="E65" s="8" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="H65" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>328</v>
-      </c>
-      <c r="D66" s="24" t="s">
-        <v>306</v>
+        <v>324</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>302</v>
       </c>
       <c r="E66" s="8" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="G66" s="19" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="H66" s="8" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="H67" s="4" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3102,511 +3059,511 @@
         <v>16</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H68" s="4" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="14" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="H69" s="4" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>17</v>
+      <c r="A70" s="25" t="s">
+        <v>356</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>18</v>
+        <v>355</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="H70" s="4" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3" t="s">
-        <v>19</v>
+      <c r="A71" s="14" t="s">
+        <v>243</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>20</v>
+        <v>242</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H71" s="4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="14" t="s">
-        <v>247</v>
+        <v>265</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c r="D72" s="7" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E72" s="8" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H72" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="14" t="s">
-        <v>269</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>270</v>
+      <c r="A73" s="17" t="s">
+        <v>353</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>352</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H73" s="4" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="17" t="s">
+      <c r="A74" s="14" t="s">
         <v>357</v>
       </c>
-      <c r="B74" s="6" t="s">
-        <v>356</v>
+      <c r="B74" s="4" t="s">
+        <v>358</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="H74" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D75" s="3" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="H75" s="4" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="B76" s="11"/>
       <c r="D76" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="G76" s="23" t="s">
-        <v>139</v>
+        <v>122</v>
+      </c>
+      <c r="G76" s="14" t="s">
+        <v>135</v>
       </c>
       <c r="H76" s="4" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="23" t="s">
-        <v>124</v>
+      <c r="A77" s="14" t="s">
+        <v>120</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="H77" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D78" s="7" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="E78" s="8" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H78" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D79" s="23" t="s">
-        <v>348</v>
+        <v>117</v>
+      </c>
+      <c r="D79" s="14" t="s">
+        <v>344</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H79" s="4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D80" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="G80" s="14" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H81" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="24" t="s">
-        <v>322</v>
+      <c r="A82" s="19" t="s">
+        <v>318</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="H82" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="19" t="s">
+        <v>315</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="G83" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="24" t="s">
-        <v>319</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>320</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="E83" s="4" t="s">
-        <v>238</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="H83" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="H84" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="H85" s="4" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H86" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="H87" s="4" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="H88" s="6" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E89" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H89" s="4" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A90" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="D90" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G89" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H89" s="4" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A90" s="20" t="s">
-        <v>341</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="E90" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="H90" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D91" s="3" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="H91" s="4" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B92" s="12"/>
       <c r="D92" s="3" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="H92" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A93" s="23" t="s">
-        <v>305</v>
+      <c r="A93" s="14" t="s">
+        <v>301</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>220</v>
-      </c>
-      <c r="G93" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="H93" s="26" t="s">
-        <v>352</v>
+        <v>216</v>
+      </c>
+      <c r="G93" t="s">
+        <v>349</v>
+      </c>
+      <c r="H93" s="20" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="G94" s="13" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="H94" s="6" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3617,342 +3574,342 @@
         <v>5</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="H95" s="4" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="E96" s="6" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E97" s="6" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H97" s="1"/>
     </row>
     <row r="98" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="H98" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="H99" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="H100" s="4" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="H101" s="6" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H102" s="4" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="H103" s="4" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="G104" s="15" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="H104" s="16" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D105" s="7" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E105" s="8" t="s">
-        <v>148</v>
-      </c>
-      <c r="G105" s="20" t="s">
-        <v>271</v>
+        <v>144</v>
+      </c>
+      <c r="G105" s="17" t="s">
+        <v>267</v>
       </c>
       <c r="H105" s="6" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="11" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="B106" s="11"/>
-      <c r="D106" s="23" t="s">
-        <v>342</v>
+      <c r="D106" s="14" t="s">
+        <v>338</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D107" s="23" t="s">
-        <v>347</v>
+        <v>165</v>
+      </c>
+      <c r="D107" s="14" t="s">
+        <v>343</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="G107" s="11" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H107" s="18"/>
     </row>
     <row r="108" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="14" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>252</v>
-      </c>
-      <c r="D108" s="23" t="s">
-        <v>237</v>
+        <v>248</v>
+      </c>
+      <c r="D108" s="14" t="s">
+        <v>233</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H108" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="23" t="s">
-        <v>245</v>
+      <c r="A109" s="14" t="s">
+        <v>241</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G109" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="H109" s="4" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A110" s="14" t="s">
+        <v>327</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="D110" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="E110" s="23" t="s">
+        <v>351</v>
+      </c>
+      <c r="G110" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="H109" s="4" t="s">
+      <c r="H110" s="4" t="s">
         <v>184</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="23" t="s">
-        <v>331</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="D110" s="30" t="s">
-        <v>354</v>
-      </c>
-      <c r="E110" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="G110" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="H110" s="4" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H111" s="4" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="H112" s="4" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
     </row>
     <row r="113" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="14" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A114" s="20" t="s">
-        <v>275</v>
+      <c r="A114" s="17" t="s">
+        <v>271</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="E114" s="6" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor: adjust cell sizing and page border
</commit_message>
<xml_diff>
--- a/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
+++ b/Settings/IntelliJ/IntelliJ-Shortcuts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-22.04\home\markus\projects\wiki\Settings\IntelliJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\markus\projects\wiki\Settings\IntelliJ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174131D5-7025-441A-BCD4-4A63D76B4CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D7A33B-EDF5-4763-A503-281D9D869A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -1290,14 +1290,14 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Schlecht" xfId="1" builtinId="27"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1328,7 +1328,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>3067050</xdr:colOff>
+      <xdr:colOff>3092823</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>44450</xdr:rowOff>
     </xdr:to>
@@ -1664,38 +1664,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P114"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A51" zoomScale="85" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="A74" sqref="A74:B74"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="G57" sqref="G57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="2.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="22.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="2.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="37.5703125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="22.5703125" style="2" customWidth="1"/>
-    <col min="10" max="10" width="30.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="4.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="2"/>
+    <col min="1" max="1" width="33.7265625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="25" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2.26953125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="41.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="24.08984375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="2.26953125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="37.54296875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="30.08984375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.54296875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="30.7265625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.453125" style="2" customWidth="1"/>
+    <col min="12" max="12" width="11.453125" style="2"/>
     <col min="13" max="13" width="24" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.85546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="41.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="43.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="11.42578125" style="2"/>
+    <col min="14" max="14" width="10.81640625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="41.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="24" t="s">
+    <row r="1" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D1" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="E1" s="24"/>
-    </row>
-    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1729,7 +1729,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>176</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>246</v>
       </c>
@@ -1769,7 +1769,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1809,7 +1809,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>139</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9" t="s">
         <v>191</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="14" t="s">
         <v>15</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>263</v>
       </c>
@@ -1909,8 +1909,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+    <row r="13" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="24" t="s">
         <v>356</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1929,7 +1929,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="14" t="s">
         <v>243</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="14" t="s">
         <v>265</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="17" t="s">
         <v>353</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
         <v>357</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D18" s="3" t="s">
         <v>162</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>114</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>120</v>
       </c>
@@ -2061,7 +2061,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
         <v>119</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>118</v>
       </c>
@@ -2101,7 +2101,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D23" s="3" t="s">
         <v>50</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>20</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="19" t="s">
         <v>318</v>
       </c>
@@ -2152,7 +2152,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="19" t="s">
         <v>315</v>
       </c>
@@ -2172,7 +2172,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3" t="s">
         <v>153</v>
       </c>
@@ -2192,7 +2192,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>21</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>200</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>150</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3" t="s">
         <v>190</v>
       </c>
@@ -2272,7 +2272,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>24</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="17" t="s">
         <v>337</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D34" s="5" t="s">
         <v>222</v>
       </c>
@@ -2324,7 +2324,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="12" t="s">
         <v>62</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="14" t="s">
         <v>301</v>
       </c>
@@ -2362,7 +2362,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>72</v>
       </c>
@@ -2382,7 +2382,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>4</v>
       </c>
@@ -2402,7 +2402,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>73</v>
       </c>
@@ -2416,7 +2416,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3" t="s">
         <v>74</v>
       </c>
@@ -2434,7 +2434,7 @@
       </c>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>75</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3" t="s">
         <v>76</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>77</v>
       </c>
@@ -2494,7 +2494,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3" t="s">
         <v>78</v>
       </c>
@@ -2514,7 +2514,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3" t="s">
         <v>79</v>
       </c>
@@ -2534,7 +2534,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>80</v>
       </c>
@@ -2553,18 +2553,18 @@
       <c r="H46" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="I46" s="24" t="s">
+      <c r="I46" s="25" t="s">
         <v>336</v>
       </c>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="24"/>
-      <c r="P46" s="24"/>
-    </row>
-    <row r="47" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
+      <c r="M46" s="25"/>
+      <c r="N46" s="25"/>
+      <c r="O46" s="25"/>
+      <c r="P46" s="25"/>
+    </row>
+    <row r="47" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3" t="s">
         <v>157</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D48" s="7" t="s">
         <v>145</v>
       </c>
@@ -2597,19 +2597,19 @@
       <c r="H48" s="6" t="s">
         <v>268</v>
       </c>
-      <c r="I48" s="24" t="s">
+      <c r="I48" s="25" t="s">
         <v>300</v>
       </c>
-      <c r="J48" s="24"/>
-      <c r="K48" s="24"/>
-      <c r="L48" s="24"/>
-      <c r="M48" s="24"/>
-      <c r="O48" s="24" t="s">
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
+      <c r="M48" s="25"/>
+      <c r="O48" s="25" t="s">
         <v>304</v>
       </c>
-      <c r="P48" s="24"/>
-    </row>
-    <row r="49" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P48" s="25"/>
+    </row>
+    <row r="49" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="11" t="s">
         <v>121</v>
       </c>
@@ -2640,7 +2640,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3" t="s">
         <v>164</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="14" t="s">
         <v>247</v>
       </c>
@@ -2710,7 +2710,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>241</v>
       </c>
@@ -2736,12 +2736,12 @@
         <v>281</v>
       </c>
       <c r="K52"/>
-      <c r="O52" s="24" t="s">
+      <c r="O52" s="25" t="s">
         <v>311</v>
       </c>
-      <c r="P52" s="24"/>
-    </row>
-    <row r="53" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="P52" s="25"/>
+    </row>
+    <row r="53" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="17" t="s">
         <v>327</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3" t="s">
         <v>143</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>156</v>
       </c>
@@ -2831,7 +2831,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="14" t="s">
         <v>257</v>
       </c>
@@ -2848,7 +2848,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="17" t="s">
         <v>271</v>
       </c>
@@ -2871,13 +2871,13 @@
         <v>314</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="24" t="s">
+    <row r="58" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="D58" s="25" t="s">
         <v>335</v>
       </c>
-      <c r="E58" s="24"/>
-    </row>
-    <row r="59" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="25"/>
+    </row>
+    <row r="59" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>6</v>
       </c>
@@ -2891,7 +2891,7 @@
       </c>
       <c r="H59" s="1"/>
     </row>
-    <row r="60" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3" t="s">
         <v>7</v>
       </c>
@@ -2911,7 +2911,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3" t="s">
         <v>176</v>
       </c>
@@ -2931,7 +2931,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>246</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3" t="s">
         <v>9</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3" t="s">
         <v>11</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3" t="s">
         <v>13</v>
       </c>
@@ -3011,7 +3011,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3" t="s">
         <v>139</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="9" t="s">
         <v>191</v>
       </c>
@@ -3051,7 +3051,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="14" t="s">
         <v>15</v>
       </c>
@@ -3071,7 +3071,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="14" t="s">
         <v>263</v>
       </c>
@@ -3091,8 +3091,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="25" t="s">
+    <row r="70" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A70" s="24" t="s">
         <v>356</v>
       </c>
       <c r="B70" s="4" t="s">
@@ -3111,7 +3111,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="14" t="s">
         <v>243</v>
       </c>
@@ -3131,7 +3131,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="14" t="s">
         <v>265</v>
       </c>
@@ -3151,7 +3151,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
         <v>353</v>
       </c>
@@ -3171,7 +3171,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="14" t="s">
         <v>357</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D75" s="3" t="s">
         <v>162</v>
       </c>
@@ -3205,7 +3205,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="11" t="s">
         <v>114</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="14" t="s">
         <v>120</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3" t="s">
         <v>119</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="7" t="s">
         <v>118</v>
       </c>
@@ -3283,7 +3283,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D80" s="3" t="s">
         <v>50</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="11" t="s">
         <v>20</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="19" t="s">
         <v>318</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="19" t="s">
         <v>315</v>
       </c>
@@ -3354,7 +3354,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3" t="s">
         <v>153</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3" t="s">
         <v>21</v>
       </c>
@@ -3394,7 +3394,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3" t="s">
         <v>200</v>
       </c>
@@ -3414,7 +3414,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3" t="s">
         <v>150</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3" t="s">
         <v>190</v>
       </c>
@@ -3454,7 +3454,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3" t="s">
         <v>24</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="17" t="s">
         <v>337</v>
       </c>
@@ -3494,7 +3494,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D91" s="3" t="s">
         <v>222</v>
       </c>
@@ -3508,7 +3508,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="12" t="s">
         <v>62</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14" t="s">
         <v>301</v>
       </c>
@@ -3546,7 +3546,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3" t="s">
         <v>72</v>
       </c>
@@ -3566,7 +3566,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>4</v>
       </c>
@@ -3586,7 +3586,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="7" t="s">
         <v>73</v>
       </c>
@@ -3600,7 +3600,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3" t="s">
         <v>74</v>
       </c>
@@ -3618,7 +3618,7 @@
       </c>
       <c r="H97" s="1"/>
     </row>
-    <row r="98" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3" t="s">
         <v>75</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3" t="s">
         <v>76</v>
       </c>
@@ -3658,7 +3658,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>77</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3" t="s">
         <v>78</v>
       </c>
@@ -3698,7 +3698,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="3" t="s">
         <v>79</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A103" s="3" t="s">
         <v>80</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="104" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A104" s="3" t="s">
         <v>157</v>
       </c>
@@ -3758,7 +3758,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="105" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="D105" s="7" t="s">
         <v>145</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A106" s="11" t="s">
         <v>121</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="107" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="3" t="s">
         <v>164</v>
       </c>
@@ -3802,7 +3802,7 @@
       </c>
       <c r="H107" s="18"/>
     </row>
-    <row r="108" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A108" s="14" t="s">
         <v>247</v>
       </c>
@@ -3822,7 +3822,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="109" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="14" t="s">
         <v>241</v>
       </c>
@@ -3842,7 +3842,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="110" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="14" t="s">
         <v>327</v>
       </c>
@@ -3862,7 +3862,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="111" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3" t="s">
         <v>143</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="112" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="3" t="s">
         <v>156</v>
       </c>
@@ -3890,7 +3890,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="113" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="14" t="s">
         <v>257</v>
       </c>
@@ -3898,7 +3898,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" s="17" t="s">
         <v>271</v>
       </c>
@@ -3921,10 +3921,10 @@
     <mergeCell ref="I46:P46"/>
     <mergeCell ref="O52:P52"/>
   </mergeCells>
-  <pageMargins left="0.39370078740157499" right="0.39370078740157499" top="0.39370078740157499" bottom="0.39370078740157499" header="0.196850393700787" footer="0.196850393700787"/>
+  <pageMargins left="0.31496062992125984" right="0.3" top="0.11811023622047245" bottom="0.35433070866141736" header="0.19685039370078741" footer="0.19685039370078741"/>
   <pageSetup paperSize="9" scale="72" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;LTool Windows: 1 Project / 2 Favorites / 3 Find / 4 Run / 5 Debug / 6 TODO / 7 Structure / 8 Services / 9 VCS / 0 Messages&amp;R&amp;"-,Fett"&amp;K00-037Shortcuts to remember &amp;K000000/&amp;K00-037 &amp;K03+027Changed or added &amp;K000000/&amp;K03+027 &amp;K06-019From Plugin</oddFooter>
+    <oddFooter>&amp;LTool Windows: 1 Project / 2 Favorites / 3 Find / 4 Run / 5 Debug / 6 TODO / 7 Structure / 8 Services / 9 VCS / 0 Messages&amp;R&amp;K00-030Shortcuts to remember&amp;K01+000 / &amp;K03+035Changed or added&amp;K01+000 / &amp;K06-020From Plugin</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>